<commit_message>
actualizacion de lista de respaldos
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Configuracion/PlanConfiguracion.xlsx
+++ b/qualtcom/Organizacional/Configuracion/PlanConfiguracion.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="117">
   <si>
     <t>Plan de Administración de Configuración</t>
   </si>
@@ -87,12 +87,6 @@
     <t>Calidad</t>
   </si>
   <si>
-    <t>Plan de auditoría</t>
-  </si>
-  <si>
-    <t>Plan_Auditoría</t>
-  </si>
-  <si>
     <t>Plan de calidad</t>
   </si>
   <si>
@@ -114,13 +108,7 @@
     <t>Auditoría Organizacional</t>
   </si>
   <si>
-    <t>PTL_Auditoría_Organizacional</t>
-  </si>
-  <si>
-    <t>Checklist de Auditoría Organizacional</t>
-  </si>
-  <si>
-    <t>Checklist Auditoría Organizacional-AAMMDD</t>
+    <t>Auditoría_Organizacional_YYMMDD</t>
   </si>
   <si>
     <t>Políticas</t>
@@ -144,28 +132,19 @@
     <t>Plan_riesgos</t>
   </si>
   <si>
-    <t>Plan de Medición</t>
-  </si>
-  <si>
-    <t>Plan_medición</t>
-  </si>
-  <si>
-    <t>Plan de Estimación</t>
-  </si>
-  <si>
-    <t>Plan_Estimación</t>
+    <t>Estimación</t>
   </si>
   <si>
     <t>Plan Estratégico</t>
   </si>
   <si>
-    <t> Plan_estratégico</t>
-  </si>
-  <si>
-    <t>Minuta de Proceso</t>
-  </si>
-  <si>
-    <t>Minuta_proceso</t>
+    <t>Plan_estratégico</t>
+  </si>
+  <si>
+    <t>Minuta de compromiso</t>
+  </si>
+  <si>
+    <t>Minuta_compromiso</t>
   </si>
   <si>
     <t>Catalogo de servicios</t>
@@ -366,9 +345,6 @@
   </si>
   <si>
     <t>Plantilla de recursos actualizado</t>
-  </si>
-  <si>
-    <t>Estimación</t>
   </si>
   <si>
     <t>WBS del proyecto (Gantt)</t>
@@ -1013,57 +989,57 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="C8" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B20" activeCellId="0" pane="topLeft" sqref="B20"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A31" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B48" activeCellId="0" pane="topLeft" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="2.74901960784314"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.0313725490196"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="47.8549019607843"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="67.0823529411765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.1372549019608"/>
-    <col collapsed="false" hidden="false" max="251" min="6" style="1" width="11.7843137254902"/>
-    <col collapsed="false" hidden="false" max="252" min="252" style="1" width="2.74901960784314"/>
-    <col collapsed="false" hidden="false" max="253" min="253" style="1" width="47.5019607843137"/>
-    <col collapsed="false" hidden="false" max="254" min="254" style="1" width="59.521568627451"/>
-    <col collapsed="false" hidden="false" max="255" min="255" style="1" width="31.3647058823529"/>
-    <col collapsed="false" hidden="false" max="256" min="256" style="1" width="11.321568627451"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="2.76862745098039"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.278431372549"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.0980392156863"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="67.4156862745098"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.2549019607843"/>
+    <col collapsed="false" hidden="false" max="251" min="6" style="1" width="11.8470588235294"/>
+    <col collapsed="false" hidden="false" max="252" min="252" style="1" width="2.76862745098039"/>
+    <col collapsed="false" hidden="false" max="253" min="253" style="1" width="47.7372549019608"/>
+    <col collapsed="false" hidden="false" max="254" min="254" style="1" width="59.8196078431373"/>
+    <col collapsed="false" hidden="false" max="255" min="255" style="1" width="31.5176470588235"/>
+    <col collapsed="false" hidden="false" max="256" min="256" style="1" width="11.3764705882353"/>
     <col collapsed="false" hidden="false" max="257" min="257" style="1" width="1.12941176470588"/>
-    <col collapsed="false" hidden="false" max="258" min="258" style="1" width="27.921568627451"/>
-    <col collapsed="false" hidden="false" max="259" min="259" style="1" width="23.1372549019608"/>
-    <col collapsed="false" hidden="false" max="260" min="260" style="1" width="2.39607843137255"/>
-    <col collapsed="false" hidden="false" max="261" min="261" style="1" width="23.1372549019608"/>
-    <col collapsed="false" hidden="false" max="507" min="262" style="1" width="11.7843137254902"/>
-    <col collapsed="false" hidden="false" max="508" min="508" style="1" width="2.74901960784314"/>
-    <col collapsed="false" hidden="false" max="509" min="509" style="1" width="47.5019607843137"/>
-    <col collapsed="false" hidden="false" max="510" min="510" style="1" width="59.521568627451"/>
-    <col collapsed="false" hidden="false" max="511" min="511" style="1" width="31.3647058823529"/>
-    <col collapsed="false" hidden="false" max="512" min="512" style="1" width="11.321568627451"/>
+    <col collapsed="false" hidden="false" max="258" min="258" style="1" width="28.0627450980392"/>
+    <col collapsed="false" hidden="false" max="259" min="259" style="1" width="23.2549019607843"/>
+    <col collapsed="false" hidden="false" max="260" min="260" style="1" width="2.40392156862745"/>
+    <col collapsed="false" hidden="false" max="261" min="261" style="1" width="23.2549019607843"/>
+    <col collapsed="false" hidden="false" max="507" min="262" style="1" width="11.8470588235294"/>
+    <col collapsed="false" hidden="false" max="508" min="508" style="1" width="2.76862745098039"/>
+    <col collapsed="false" hidden="false" max="509" min="509" style="1" width="47.7372549019608"/>
+    <col collapsed="false" hidden="false" max="510" min="510" style="1" width="59.8196078431373"/>
+    <col collapsed="false" hidden="false" max="511" min="511" style="1" width="31.5176470588235"/>
+    <col collapsed="false" hidden="false" max="512" min="512" style="1" width="11.3764705882353"/>
     <col collapsed="false" hidden="false" max="513" min="513" style="1" width="1.12941176470588"/>
-    <col collapsed="false" hidden="false" max="514" min="514" style="1" width="27.921568627451"/>
-    <col collapsed="false" hidden="false" max="515" min="515" style="1" width="23.1372549019608"/>
-    <col collapsed="false" hidden="false" max="516" min="516" style="1" width="2.39607843137255"/>
-    <col collapsed="false" hidden="false" max="517" min="517" style="1" width="23.1372549019608"/>
-    <col collapsed="false" hidden="false" max="763" min="518" style="1" width="11.7843137254902"/>
-    <col collapsed="false" hidden="false" max="764" min="764" style="1" width="2.74901960784314"/>
-    <col collapsed="false" hidden="false" max="765" min="765" style="1" width="47.5019607843137"/>
-    <col collapsed="false" hidden="false" max="766" min="766" style="1" width="59.521568627451"/>
-    <col collapsed="false" hidden="false" max="767" min="767" style="1" width="31.3647058823529"/>
-    <col collapsed="false" hidden="false" max="768" min="768" style="1" width="11.321568627451"/>
+    <col collapsed="false" hidden="false" max="514" min="514" style="1" width="28.0627450980392"/>
+    <col collapsed="false" hidden="false" max="515" min="515" style="1" width="23.2549019607843"/>
+    <col collapsed="false" hidden="false" max="516" min="516" style="1" width="2.40392156862745"/>
+    <col collapsed="false" hidden="false" max="517" min="517" style="1" width="23.2549019607843"/>
+    <col collapsed="false" hidden="false" max="763" min="518" style="1" width="11.8470588235294"/>
+    <col collapsed="false" hidden="false" max="764" min="764" style="1" width="2.76862745098039"/>
+    <col collapsed="false" hidden="false" max="765" min="765" style="1" width="47.7372549019608"/>
+    <col collapsed="false" hidden="false" max="766" min="766" style="1" width="59.8196078431373"/>
+    <col collapsed="false" hidden="false" max="767" min="767" style="1" width="31.5176470588235"/>
+    <col collapsed="false" hidden="false" max="768" min="768" style="1" width="11.3764705882353"/>
     <col collapsed="false" hidden="false" max="769" min="769" style="1" width="1.12941176470588"/>
-    <col collapsed="false" hidden="false" max="770" min="770" style="1" width="27.921568627451"/>
-    <col collapsed="false" hidden="false" max="771" min="771" style="1" width="23.1372549019608"/>
-    <col collapsed="false" hidden="false" max="772" min="772" style="1" width="2.39607843137255"/>
-    <col collapsed="false" hidden="false" max="773" min="773" style="1" width="23.1372549019608"/>
-    <col collapsed="false" hidden="false" max="1019" min="774" style="1" width="11.7843137254902"/>
-    <col collapsed="false" hidden="false" max="1020" min="1020" style="1" width="2.74901960784314"/>
-    <col collapsed="false" hidden="false" max="1021" min="1021" style="1" width="47.5019607843137"/>
-    <col collapsed="false" hidden="false" max="1022" min="1022" style="1" width="59.521568627451"/>
-    <col collapsed="false" hidden="false" max="1023" min="1023" style="1" width="31.3647058823529"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="11.321568627451"/>
+    <col collapsed="false" hidden="false" max="770" min="770" style="1" width="28.0627450980392"/>
+    <col collapsed="false" hidden="false" max="771" min="771" style="1" width="23.2549019607843"/>
+    <col collapsed="false" hidden="false" max="772" min="772" style="1" width="2.40392156862745"/>
+    <col collapsed="false" hidden="false" max="773" min="773" style="1" width="23.2549019607843"/>
+    <col collapsed="false" hidden="false" max="1019" min="774" style="1" width="11.8470588235294"/>
+    <col collapsed="false" hidden="false" max="1020" min="1020" style="1" width="2.76862745098039"/>
+    <col collapsed="false" hidden="false" max="1021" min="1021" style="1" width="47.7372549019608"/>
+    <col collapsed="false" hidden="false" max="1022" min="1022" style="1" width="59.8196078431373"/>
+    <col collapsed="false" hidden="false" max="1023" min="1023" style="1" width="31.5176470588235"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="11.3764705882353"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="1">
@@ -1217,22 +1193,22 @@
       <c r="B16" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="14" t="s">
-        <v>7</v>
-      </c>
+      <c r="D16" s="14"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="17">
       <c r="A17" s="6"/>
       <c r="B17" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="14"/>
+      <c r="D17" s="14" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="18">
       <c r="A18" s="6"/>
@@ -1242,9 +1218,7 @@
       <c r="C18" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>7</v>
-      </c>
+      <c r="D18" s="14"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="19">
       <c r="A19" s="6"/>
@@ -1258,21 +1232,19 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="20">
       <c r="A20" s="6"/>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="14"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="23"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="21">
       <c r="A21" s="6"/>
       <c r="B21" s="27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>7</v>
@@ -1280,341 +1252,342 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="22">
       <c r="A22" s="6"/>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="23" s="30">
+      <c r="B23" s="31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
+      <c r="B24" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
+      <c r="B25" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="C22" s="22"/>
-      <c r="D22" s="23"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="23">
-      <c r="A23" s="6"/>
-      <c r="B23" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="14" t="s">
+      <c r="C25" s="33"/>
+      <c r="D25" s="34"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
+      <c r="B26" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="24">
-      <c r="A24" s="6"/>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="25" s="30">
-      <c r="B25" s="31" t="s">
+      <c r="C26" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
-      <c r="B26" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="28"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
+      <c r="B27" s="27" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
-      <c r="B27" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="34"/>
+      <c r="C27" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="28"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="28">
       <c r="B28" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="28" t="s">
         <v>38</v>
-      </c>
-      <c r="C28" s="28" t="s">
-        <v>39</v>
       </c>
       <c r="D28" s="28"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="29">
       <c r="B29" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="28" t="s">
         <v>40</v>
-      </c>
-      <c r="C29" s="28" t="s">
-        <v>41</v>
       </c>
       <c r="D29" s="28"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
       <c r="B30" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="D30" s="28"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
+      <c r="B31" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="D30" s="28"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
-      <c r="B31" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="28"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="34"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
       <c r="B32" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C32" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="36"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="2" r="33">
+      <c r="B33" s="37"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="38"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="16.5" outlineLevel="0" r="34" s="30">
+      <c r="B34" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="16.5" outlineLevel="0" r="35" s="30">
+      <c r="B35" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="16.5" outlineLevel="0" r="36" s="30">
+      <c r="B36" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="40"/>
+      <c r="D36" s="41"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="16.5" outlineLevel="0" r="37" s="30">
+      <c r="B37" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="43"/>
+      <c r="D37" s="44"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="16.5" outlineLevel="0" r="38" s="30">
+      <c r="B38" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="D32" s="28"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
-      <c r="B33" s="27" t="s">
+      <c r="D38" s="36"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="16.5" outlineLevel="0" r="39" s="30">
+      <c r="B39" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C39" s="46"/>
+      <c r="D39" s="47"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="true" ht="16.5" outlineLevel="0" r="40" s="30">
+      <c r="B40" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="28"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="34">
-      <c r="B34" s="35" t="s">
+      <c r="D40" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="41" s="30">
+      <c r="B41" s="49"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
+      <c r="B42" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="34"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="35">
-      <c r="B35" s="27" t="s">
+      <c r="C42" s="31"/>
+      <c r="D42" s="31"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="43">
+      <c r="B43" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C43" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="D35" s="36"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="2" r="36">
-      <c r="B36" s="37"/>
-      <c r="C36" s="37"/>
-      <c r="D36" s="38"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="37" s="30">
-      <c r="B37" s="31" t="s">
+      <c r="D43" s="50" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="38" s="30">
-      <c r="B38" s="39" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="39" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="44">
+      <c r="B44" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="52"/>
+      <c r="D44" s="53"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="45">
+      <c r="B45" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="46">
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="38"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="47">
+      <c r="A47" s="56"/>
+      <c r="B47" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="39" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="39" s="30">
-      <c r="B39" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C39" s="40"/>
-      <c r="D39" s="41"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="40" s="30">
-      <c r="B40" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="C40" s="43"/>
-      <c r="D40" s="44"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="41" s="30">
-      <c r="B41" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C41" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="D41" s="36"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="42" s="30">
-      <c r="B42" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="C42" s="46"/>
-      <c r="D42" s="47"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="43" s="30">
-      <c r="B43" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C43" s="48" t="s">
+      <c r="C47" s="9"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="48">
+      <c r="B48" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D43" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="44" s="30">
-      <c r="B44" s="49"/>
-      <c r="C44" s="49"/>
-      <c r="D44" s="49"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="45">
-      <c r="B45" s="31" t="s">
+      <c r="C48" s="58"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="49">
+      <c r="B49" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="C45" s="31"/>
-      <c r="D45" s="31"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="46">
-      <c r="B46" s="50" t="s">
+      <c r="C49" s="60"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
+      <c r="B50" s="61"/>
+      <c r="C50" s="62"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="51">
+      <c r="B51" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="50" t="s">
+      <c r="C51" s="62"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
+      <c r="B52" s="64"/>
+      <c r="C52" s="65"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="53">
+      <c r="A53" s="56"/>
+      <c r="B53" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="D46" s="50" t="s">
+      <c r="C53" s="10"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="1" r="54">
+      <c r="B54" s="67" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="47">
-      <c r="B47" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="52"/>
-      <c r="D47" s="53"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="48">
-      <c r="B48" s="54" t="s">
-        <v>37</v>
-      </c>
-      <c r="C48" s="54" t="s">
+      <c r="C54" s="68"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="1" r="55">
+      <c r="B55" s="69"/>
+      <c r="C55" s="69"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="1" r="56">
+      <c r="B56" s="69"/>
+      <c r="C56" s="69"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
+      <c r="A57" s="65"/>
+      <c r="B57" s="70"/>
+      <c r="C57" s="65"/>
+      <c r="D57" s="65"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
+      <c r="B58" s="71"/>
+      <c r="C58" s="65"/>
+      <c r="D58" s="65"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
+      <c r="B59" s="65"/>
+      <c r="C59" s="65"/>
+      <c r="D59" s="65"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="60">
+      <c r="A60" s="56"/>
+      <c r="B60" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="D48" s="55" t="s">
+      <c r="C60" s="66" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="49">
-      <c r="B49" s="37"/>
-      <c r="C49" s="37"/>
-      <c r="D49" s="38"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="50">
-      <c r="A50" s="56"/>
-      <c r="B50" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C50" s="9"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="51">
-      <c r="B51" s="57" t="s">
+      <c r="D60" s="66" t="s">
         <v>63</v>
       </c>
-      <c r="C51" s="58"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="52">
-      <c r="B52" s="59" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
+      <c r="B61" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="C52" s="60"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
-      <c r="B53" s="61"/>
-      <c r="C53" s="62"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="54">
-      <c r="B54" s="63" t="s">
+      <c r="C61" s="72"/>
+      <c r="D61" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="C54" s="62"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
-      <c r="B55" s="64"/>
-      <c r="C55" s="65"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="56">
-      <c r="A56" s="56"/>
-      <c r="B56" s="66" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="62">
+      <c r="B62" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="C56" s="10"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="1" r="57">
-      <c r="B57" s="67" t="s">
+      <c r="C62" s="72" t="s">
         <v>67</v>
       </c>
-      <c r="C57" s="68"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="1" r="58">
-      <c r="B58" s="69"/>
-      <c r="C58" s="69"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="1" r="59">
-      <c r="B59" s="69"/>
-      <c r="C59" s="69"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
-      <c r="A60" s="65"/>
-      <c r="B60" s="70"/>
-      <c r="C60" s="65"/>
-      <c r="D60" s="65"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
-      <c r="B61" s="71"/>
-      <c r="C61" s="65"/>
-      <c r="D61" s="65"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
-      <c r="B62" s="65"/>
-      <c r="C62" s="65"/>
-      <c r="D62" s="65"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="63">
-      <c r="A63" s="56"/>
-      <c r="B63" s="66" t="s">
+      <c r="D62" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="C63" s="66" t="s">
-        <v>69</v>
-      </c>
-      <c r="D63" s="66" t="s">
-        <v>70</v>
-      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
+      <c r="B63" s="69"/>
+      <c r="C63" s="69"/>
+      <c r="D63" s="69"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
-      <c r="B64" s="72" t="s">
-        <v>71</v>
-      </c>
-      <c r="C64" s="72"/>
-      <c r="D64" s="72" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="65">
-      <c r="B65" s="72" t="s">
-        <v>73</v>
-      </c>
-      <c r="C65" s="72" t="s">
-        <v>74</v>
-      </c>
-      <c r="D65" s="73" t="s">
-        <v>75</v>
-      </c>
+      <c r="B64" s="65"/>
+      <c r="C64" s="65"/>
+      <c r="D64" s="65"/>
+      <c r="E64" s="65"/>
+      <c r="F64" s="65"/>
+      <c r="G64" s="65"/>
+      <c r="H64" s="65"/>
+      <c r="I64" s="65"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
+      <c r="B65" s="65"/>
+      <c r="C65" s="65"/>
+      <c r="D65" s="65"/>
+      <c r="E65" s="65"/>
+      <c r="F65" s="65"/>
+      <c r="G65" s="65"/>
+      <c r="H65" s="65"/>
+      <c r="I65" s="65"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
-      <c r="B66" s="69"/>
-      <c r="C66" s="69"/>
-      <c r="D66" s="69"/>
+      <c r="B66" s="65"/>
+      <c r="C66" s="65"/>
+      <c r="D66" s="65"/>
+      <c r="E66" s="65"/>
+      <c r="F66" s="65"/>
+      <c r="G66" s="65"/>
+      <c r="H66" s="65"/>
+      <c r="I66" s="65"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
       <c r="B67" s="65"/>
@@ -2026,42 +1999,12 @@
       <c r="H107" s="65"/>
       <c r="I107" s="65"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="108">
-      <c r="B108" s="65"/>
-      <c r="C108" s="65"/>
-      <c r="D108" s="65"/>
-      <c r="E108" s="65"/>
-      <c r="F108" s="65"/>
-      <c r="G108" s="65"/>
-      <c r="H108" s="65"/>
-      <c r="I108" s="65"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="109">
-      <c r="B109" s="65"/>
-      <c r="C109" s="65"/>
-      <c r="D109" s="65"/>
-      <c r="E109" s="65"/>
-      <c r="F109" s="65"/>
-      <c r="G109" s="65"/>
-      <c r="H109" s="65"/>
-      <c r="I109" s="65"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="110">
-      <c r="B110" s="65"/>
-      <c r="C110" s="65"/>
-      <c r="D110" s="65"/>
-      <c r="E110" s="65"/>
-      <c r="F110" s="65"/>
-      <c r="G110" s="65"/>
-      <c r="H110" s="65"/>
-      <c r="I110" s="65"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B42:D42"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2085,46 +2028,46 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7843137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.1333333333333"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.2470588235294"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.5686274509804"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.3647058823529"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="39.8392156862745"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.4901960784314"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.4470588235294"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="40.6352941176471"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.7843137254902"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.5333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.7843137254902"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8470588235294"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.3607843137255"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.4"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.7764705882353"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.4823529411765"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.0392156862745"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.6705882352941"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.5803921568627"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="40.843137254902"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.8470588235294"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.6078431372549"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.8470588235294"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="B2" s="0" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
       <c r="A5" s="74" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B5" s="74" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C5" s="74" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D5" s="74" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E5" s="74" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="F5" s="74" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="G5" s="74" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="H5" s="74" t="s">
         <v>8</v>
@@ -2138,122 +2081,122 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
       <c r="A6" s="74" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" s="74" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="74" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="74" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="74" t="s">
+        <v>82</v>
+      </c>
+      <c r="H6" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="B6" s="74" t="s">
+      <c r="I6" s="74" t="s">
         <v>84</v>
-      </c>
-      <c r="C6" s="74" t="s">
-        <v>85</v>
-      </c>
-      <c r="D6" s="74" t="s">
-        <v>86</v>
-      </c>
-      <c r="E6" s="74" t="s">
-        <v>87</v>
-      </c>
-      <c r="F6" s="74" t="s">
-        <v>88</v>
-      </c>
-      <c r="G6" s="74" t="s">
-        <v>89</v>
-      </c>
-      <c r="H6" s="74" t="s">
-        <v>90</v>
-      </c>
-      <c r="I6" s="74" t="s">
-        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
       <c r="B7" s="75" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C7" s="76" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D7" s="75" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="E7" s="77" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F7" s="76" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G7" s="76" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="H7" s="76" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="I7" s="78" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
       <c r="B8" s="75" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="C8" s="76" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D8" s="75" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E8" s="75" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F8" s="75" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H8" s="76" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="I8" s="78" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
       <c r="B9" s="75" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C9" s="76" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D9" s="75" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E9" s="77" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="F9" s="75" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="I9" s="78" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
       <c r="B10" s="76" t="s">
-        <v>111</v>
+        <v>36</v>
       </c>
       <c r="C10" s="76" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="I10" s="78" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
       <c r="B11" s="76" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C11" s="76" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="I11" s="79" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>51</v>
@@ -2261,13 +2204,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
       <c r="B12" s="76" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C12" s="76" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="I12" s="79" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>50</v>
@@ -2275,18 +2218,18 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
       <c r="B13" s="76" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="I13" s="79" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="B14" s="76" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="I14" s="79" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
@@ -2296,12 +2239,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="B19" s="75" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="B20" s="77" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
integracion de diagrama organizacional
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Configuracion/PlanConfiguracion.xlsx
+++ b/qualtcom/Organizacional/Configuracion/PlanConfiguracion.xlsx
@@ -753,7 +753,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
@@ -774,6 +774,9 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="6" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="5" fontId="11" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="6" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
@@ -797,7 +800,7 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="6" fontId="11" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="6" fontId="11" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="5" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="5" fontId="12" numFmtId="164" xfId="0"/>
@@ -812,6 +815,9 @@
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="4" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="6" fontId="11" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="5" fontId="14" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="13" numFmtId="164" xfId="0">
@@ -977,55 +983,55 @@
   </sheetPr>
   <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A47" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C55" activeCellId="0" pane="topLeft" sqref="C55"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A32" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C36" activeCellId="0" pane="topLeft" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="2.7843137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.5294117647059"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.3333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="67.7529411764706"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.3686274509804"/>
-    <col collapsed="false" hidden="false" max="251" min="6" style="1" width="11.9019607843137"/>
-    <col collapsed="false" hidden="false" max="252" min="252" style="1" width="2.7843137254902"/>
-    <col collapsed="false" hidden="false" max="253" min="253" style="1" width="47.9803921568627"/>
-    <col collapsed="false" hidden="false" max="254" min="254" style="1" width="60.1176470588235"/>
-    <col collapsed="false" hidden="false" max="255" min="255" style="1" width="31.6745098039216"/>
-    <col collapsed="false" hidden="false" max="256" min="256" style="1" width="11.4313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="2.80392156862745"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.7843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.5764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="68.0941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.4862745098039"/>
+    <col collapsed="false" hidden="false" max="251" min="6" style="1" width="11.9647058823529"/>
+    <col collapsed="false" hidden="false" max="252" min="252" style="1" width="2.80392156862745"/>
+    <col collapsed="false" hidden="false" max="253" min="253" style="1" width="48.2156862745098"/>
+    <col collapsed="false" hidden="false" max="254" min="254" style="1" width="60.4156862745098"/>
+    <col collapsed="false" hidden="false" max="255" min="255" style="1" width="31.8274509803922"/>
+    <col collapsed="false" hidden="false" max="256" min="256" style="1" width="11.4862745098039"/>
     <col collapsed="false" hidden="false" max="257" min="257" style="1" width="1.12941176470588"/>
-    <col collapsed="false" hidden="false" max="258" min="258" style="1" width="28.2"/>
-    <col collapsed="false" hidden="false" max="259" min="259" style="1" width="23.3686274509804"/>
-    <col collapsed="false" hidden="false" max="260" min="260" style="1" width="2.4156862745098"/>
-    <col collapsed="false" hidden="false" max="261" min="261" style="1" width="23.3686274509804"/>
-    <col collapsed="false" hidden="false" max="507" min="262" style="1" width="11.9019607843137"/>
-    <col collapsed="false" hidden="false" max="508" min="508" style="1" width="2.7843137254902"/>
-    <col collapsed="false" hidden="false" max="509" min="509" style="1" width="47.9803921568627"/>
-    <col collapsed="false" hidden="false" max="510" min="510" style="1" width="60.1176470588235"/>
-    <col collapsed="false" hidden="false" max="511" min="511" style="1" width="31.6745098039216"/>
-    <col collapsed="false" hidden="false" max="512" min="512" style="1" width="11.4313725490196"/>
+    <col collapsed="false" hidden="false" max="258" min="258" style="1" width="28.3372549019608"/>
+    <col collapsed="false" hidden="false" max="259" min="259" style="1" width="23.4862745098039"/>
+    <col collapsed="false" hidden="false" max="260" min="260" style="1" width="2.42352941176471"/>
+    <col collapsed="false" hidden="false" max="261" min="261" style="1" width="23.4862745098039"/>
+    <col collapsed="false" hidden="false" max="507" min="262" style="1" width="11.9647058823529"/>
+    <col collapsed="false" hidden="false" max="508" min="508" style="1" width="2.80392156862745"/>
+    <col collapsed="false" hidden="false" max="509" min="509" style="1" width="48.2156862745098"/>
+    <col collapsed="false" hidden="false" max="510" min="510" style="1" width="60.4156862745098"/>
+    <col collapsed="false" hidden="false" max="511" min="511" style="1" width="31.8274509803922"/>
+    <col collapsed="false" hidden="false" max="512" min="512" style="1" width="11.4862745098039"/>
     <col collapsed="false" hidden="false" max="513" min="513" style="1" width="1.12941176470588"/>
-    <col collapsed="false" hidden="false" max="514" min="514" style="1" width="28.2"/>
-    <col collapsed="false" hidden="false" max="515" min="515" style="1" width="23.3686274509804"/>
-    <col collapsed="false" hidden="false" max="516" min="516" style="1" width="2.4156862745098"/>
-    <col collapsed="false" hidden="false" max="517" min="517" style="1" width="23.3686274509804"/>
-    <col collapsed="false" hidden="false" max="763" min="518" style="1" width="11.9019607843137"/>
-    <col collapsed="false" hidden="false" max="764" min="764" style="1" width="2.7843137254902"/>
-    <col collapsed="false" hidden="false" max="765" min="765" style="1" width="47.9803921568627"/>
-    <col collapsed="false" hidden="false" max="766" min="766" style="1" width="60.1176470588235"/>
-    <col collapsed="false" hidden="false" max="767" min="767" style="1" width="31.6745098039216"/>
-    <col collapsed="false" hidden="false" max="768" min="768" style="1" width="11.4313725490196"/>
+    <col collapsed="false" hidden="false" max="514" min="514" style="1" width="28.3372549019608"/>
+    <col collapsed="false" hidden="false" max="515" min="515" style="1" width="23.4862745098039"/>
+    <col collapsed="false" hidden="false" max="516" min="516" style="1" width="2.42352941176471"/>
+    <col collapsed="false" hidden="false" max="517" min="517" style="1" width="23.4862745098039"/>
+    <col collapsed="false" hidden="false" max="763" min="518" style="1" width="11.9647058823529"/>
+    <col collapsed="false" hidden="false" max="764" min="764" style="1" width="2.80392156862745"/>
+    <col collapsed="false" hidden="false" max="765" min="765" style="1" width="48.2156862745098"/>
+    <col collapsed="false" hidden="false" max="766" min="766" style="1" width="60.4156862745098"/>
+    <col collapsed="false" hidden="false" max="767" min="767" style="1" width="31.8274509803922"/>
+    <col collapsed="false" hidden="false" max="768" min="768" style="1" width="11.4862745098039"/>
     <col collapsed="false" hidden="false" max="769" min="769" style="1" width="1.12941176470588"/>
-    <col collapsed="false" hidden="false" max="770" min="770" style="1" width="28.2"/>
-    <col collapsed="false" hidden="false" max="771" min="771" style="1" width="23.3686274509804"/>
-    <col collapsed="false" hidden="false" max="772" min="772" style="1" width="2.4156862745098"/>
-    <col collapsed="false" hidden="false" max="773" min="773" style="1" width="23.3686274509804"/>
-    <col collapsed="false" hidden="false" max="1019" min="774" style="1" width="11.9019607843137"/>
-    <col collapsed="false" hidden="false" max="1020" min="1020" style="1" width="2.7843137254902"/>
-    <col collapsed="false" hidden="false" max="1021" min="1021" style="1" width="47.9803921568627"/>
-    <col collapsed="false" hidden="false" max="1022" min="1022" style="1" width="60.1176470588235"/>
-    <col collapsed="false" hidden="false" max="1023" min="1023" style="1" width="31.6745098039216"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="11.4313725490196"/>
+    <col collapsed="false" hidden="false" max="770" min="770" style="1" width="28.3372549019608"/>
+    <col collapsed="false" hidden="false" max="771" min="771" style="1" width="23.4862745098039"/>
+    <col collapsed="false" hidden="false" max="772" min="772" style="1" width="2.42352941176471"/>
+    <col collapsed="false" hidden="false" max="773" min="773" style="1" width="23.4862745098039"/>
+    <col collapsed="false" hidden="false" max="1019" min="774" style="1" width="11.9647058823529"/>
+    <col collapsed="false" hidden="false" max="1020" min="1020" style="1" width="2.80392156862745"/>
+    <col collapsed="false" hidden="false" max="1021" min="1021" style="1" width="48.2156862745098"/>
+    <col collapsed="false" hidden="false" max="1022" min="1022" style="1" width="60.4156862745098"/>
+    <col collapsed="false" hidden="false" max="1023" min="1023" style="1" width="31.8274509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="11.4862745098039"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="1">
@@ -1078,17 +1084,17 @@
       <c r="C6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="7">
       <c r="A7" s="6"/>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="18"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="8">
       <c r="A8" s="6"/>
@@ -1098,27 +1104,27 @@
       <c r="C8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="9">
       <c r="A9" s="6"/>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="10">
       <c r="A10" s="6"/>
       <c r="B10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="15" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1127,10 +1133,10 @@
       <c r="B11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="15" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1139,10 +1145,10 @@
       <c r="B12" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="15" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1154,152 +1160,152 @@
       <c r="C13" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="14">
       <c r="A14" s="6"/>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="24"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="15">
       <c r="A15" s="6"/>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D15" s="14"/>
+      <c r="D15" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="16">
       <c r="A16" s="6"/>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="17">
       <c r="A17" s="6"/>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="25" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="14"/>
+      <c r="D17" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="18">
       <c r="A18" s="6"/>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="19">
       <c r="A19" s="6"/>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="25" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="20">
       <c r="A20" s="6"/>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="14"/>
+      <c r="D20" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="21">
       <c r="A21" s="6"/>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="31"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="25"/>
+      <c r="D22" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="25"/>
+      <c r="D23" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="25"/>
+      <c r="D24" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="25"/>
+      <c r="D25" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="33"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="35"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="34"/>
+      <c r="D27" s="36"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="28">
       <c r="A28" s="6"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="29" s="36">
-      <c r="B29" s="37" t="s">
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="29" s="38">
+      <c r="B29" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
       <c r="B30" s="12" t="s">
@@ -1313,676 +1319,676 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="32"/>
-      <c r="D31" s="33"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="35"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="25" t="s">
+      <c r="C32" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="25"/>
+      <c r="D32" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
-      <c r="B33" s="24" t="s">
+      <c r="B33" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="25" t="s">
+      <c r="C33" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="25"/>
+      <c r="D33" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="34">
-      <c r="B34" s="24" t="s">
+      <c r="B34" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="25" t="s">
+      <c r="C34" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="25"/>
+      <c r="D34" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="35">
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="25"/>
+      <c r="D35" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
-      <c r="B36" s="24" t="s">
+      <c r="B36" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="25"/>
+      <c r="D36" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="37">
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="33" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="32"/>
-      <c r="D37" s="33"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="35"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
-      <c r="B38" s="24" t="s">
+      <c r="B38" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="25" t="s">
+      <c r="C38" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="D38" s="34"/>
+      <c r="D38" s="36"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="39">
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="32"/>
-      <c r="D39" s="33"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="35"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="40">
       <c r="A40" s="6"/>
-      <c r="B40" s="24" t="s">
+      <c r="B40" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="14" t="s">
+      <c r="D40" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="41" s="36">
-      <c r="B41" s="39"/>
-      <c r="C41" s="39"/>
-      <c r="D41" s="39"/>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="41" s="38">
+      <c r="B41" s="41"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="37"/>
-      <c r="D42" s="37"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="43">
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="40" t="s">
+      <c r="C43" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="D43" s="40" t="s">
+      <c r="D43" s="42" t="s">
         <v>55</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="44">
-      <c r="B44" s="41" t="s">
+      <c r="B44" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="42"/>
-      <c r="D44" s="43"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="45"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="45">
-      <c r="B45" s="44" t="s">
+      <c r="B45" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="44" t="s">
+      <c r="C45" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="45" t="s">
+      <c r="D45" s="47" t="s">
         <v>57</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="46">
-      <c r="B46" s="46"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="47"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="48"/>
+      <c r="D46" s="49"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="47">
-      <c r="A47" s="48"/>
+      <c r="A47" s="50"/>
       <c r="B47" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C47" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="48">
-      <c r="B48" s="49" t="s">
+      <c r="B48" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="50"/>
+      <c r="C48" s="52"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="49">
-      <c r="B49" s="51" t="s">
+      <c r="B49" s="53" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="52"/>
+      <c r="C49" s="54"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
-      <c r="B50" s="53"/>
-      <c r="C50" s="54"/>
+      <c r="B50" s="55"/>
+      <c r="C50" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="51">
-      <c r="A51" s="48"/>
-      <c r="B51" s="55" t="s">
+      <c r="A51" s="50"/>
+      <c r="B51" s="57" t="s">
         <v>60</v>
       </c>
       <c r="C51" s="10"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="1" r="52">
-      <c r="B52" s="56" t="s">
+      <c r="B52" s="58" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="57"/>
+      <c r="C52" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="1" r="53">
-      <c r="B53" s="58"/>
-      <c r="C53" s="58"/>
+      <c r="B53" s="60"/>
+      <c r="C53" s="60"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="1" r="54">
-      <c r="B54" s="58"/>
-      <c r="C54" s="58"/>
+      <c r="B54" s="60"/>
+      <c r="C54" s="60"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
-      <c r="A55" s="54"/>
-      <c r="B55" s="59"/>
-      <c r="C55" s="54"/>
-      <c r="D55" s="54"/>
+      <c r="A55" s="56"/>
+      <c r="B55" s="61"/>
+      <c r="C55" s="56"/>
+      <c r="D55" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
-      <c r="B56" s="60"/>
-      <c r="C56" s="54"/>
-      <c r="D56" s="54"/>
+      <c r="B56" s="62"/>
+      <c r="C56" s="56"/>
+      <c r="D56" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
-      <c r="B57" s="54"/>
-      <c r="C57" s="54"/>
-      <c r="D57" s="54"/>
+      <c r="B57" s="56"/>
+      <c r="C57" s="56"/>
+      <c r="D57" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="58">
-      <c r="A58" s="48"/>
-      <c r="B58" s="55" t="s">
+      <c r="A58" s="50"/>
+      <c r="B58" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="C58" s="55" t="s">
+      <c r="C58" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="D58" s="55" t="s">
+      <c r="D58" s="57" t="s">
         <v>64</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
-      <c r="B59" s="61" t="s">
+      <c r="B59" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="C59" s="61" t="s">
+      <c r="C59" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="D59" s="61" t="s">
+      <c r="D59" s="63" t="s">
         <v>67</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="60">
-      <c r="B60" s="61" t="s">
+      <c r="B60" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="C60" s="61" t="s">
+      <c r="C60" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="D60" s="62" t="s">
+      <c r="D60" s="64" t="s">
         <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
-      <c r="B61" s="58"/>
-      <c r="C61" s="58"/>
-      <c r="D61" s="58"/>
+      <c r="B61" s="60"/>
+      <c r="C61" s="60"/>
+      <c r="D61" s="60"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
-      <c r="B62" s="54"/>
-      <c r="C62" s="54"/>
-      <c r="D62" s="54"/>
-      <c r="E62" s="54"/>
-      <c r="F62" s="54"/>
-      <c r="G62" s="54"/>
-      <c r="H62" s="54"/>
-      <c r="I62" s="54"/>
+      <c r="B62" s="56"/>
+      <c r="C62" s="56"/>
+      <c r="D62" s="56"/>
+      <c r="E62" s="56"/>
+      <c r="F62" s="56"/>
+      <c r="G62" s="56"/>
+      <c r="H62" s="56"/>
+      <c r="I62" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
-      <c r="B63" s="54"/>
-      <c r="C63" s="54"/>
-      <c r="D63" s="54"/>
-      <c r="E63" s="54"/>
-      <c r="F63" s="54"/>
-      <c r="G63" s="54"/>
-      <c r="H63" s="54"/>
-      <c r="I63" s="54"/>
+      <c r="B63" s="56"/>
+      <c r="C63" s="56"/>
+      <c r="D63" s="56"/>
+      <c r="E63" s="56"/>
+      <c r="F63" s="56"/>
+      <c r="G63" s="56"/>
+      <c r="H63" s="56"/>
+      <c r="I63" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
-      <c r="B64" s="54"/>
-      <c r="C64" s="54"/>
-      <c r="D64" s="54"/>
-      <c r="E64" s="54"/>
-      <c r="F64" s="54"/>
-      <c r="G64" s="54"/>
-      <c r="H64" s="54"/>
-      <c r="I64" s="54"/>
+      <c r="B64" s="56"/>
+      <c r="C64" s="56"/>
+      <c r="D64" s="56"/>
+      <c r="E64" s="56"/>
+      <c r="F64" s="56"/>
+      <c r="G64" s="56"/>
+      <c r="H64" s="56"/>
+      <c r="I64" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
-      <c r="B65" s="54"/>
-      <c r="C65" s="54"/>
-      <c r="D65" s="54"/>
-      <c r="E65" s="54"/>
-      <c r="F65" s="54"/>
-      <c r="G65" s="54"/>
-      <c r="H65" s="54"/>
-      <c r="I65" s="54"/>
+      <c r="B65" s="56"/>
+      <c r="C65" s="56"/>
+      <c r="D65" s="56"/>
+      <c r="E65" s="56"/>
+      <c r="F65" s="56"/>
+      <c r="G65" s="56"/>
+      <c r="H65" s="56"/>
+      <c r="I65" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
-      <c r="B66" s="54"/>
-      <c r="C66" s="54"/>
-      <c r="D66" s="54"/>
-      <c r="E66" s="54"/>
-      <c r="F66" s="54"/>
-      <c r="G66" s="54"/>
-      <c r="H66" s="54"/>
-      <c r="I66" s="54"/>
+      <c r="B66" s="56"/>
+      <c r="C66" s="56"/>
+      <c r="D66" s="56"/>
+      <c r="E66" s="56"/>
+      <c r="F66" s="56"/>
+      <c r="G66" s="56"/>
+      <c r="H66" s="56"/>
+      <c r="I66" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
-      <c r="B67" s="54"/>
-      <c r="C67" s="54"/>
-      <c r="D67" s="54"/>
-      <c r="E67" s="54"/>
-      <c r="F67" s="54"/>
-      <c r="G67" s="54"/>
-      <c r="H67" s="54"/>
-      <c r="I67" s="54"/>
+      <c r="B67" s="56"/>
+      <c r="C67" s="56"/>
+      <c r="D67" s="56"/>
+      <c r="E67" s="56"/>
+      <c r="F67" s="56"/>
+      <c r="G67" s="56"/>
+      <c r="H67" s="56"/>
+      <c r="I67" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
-      <c r="B68" s="54"/>
-      <c r="C68" s="54"/>
-      <c r="D68" s="54"/>
-      <c r="E68" s="54"/>
-      <c r="F68" s="54"/>
-      <c r="G68" s="54"/>
-      <c r="H68" s="54"/>
-      <c r="I68" s="54"/>
+      <c r="B68" s="56"/>
+      <c r="C68" s="56"/>
+      <c r="D68" s="56"/>
+      <c r="E68" s="56"/>
+      <c r="F68" s="56"/>
+      <c r="G68" s="56"/>
+      <c r="H68" s="56"/>
+      <c r="I68" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
-      <c r="B69" s="54"/>
-      <c r="C69" s="54"/>
-      <c r="D69" s="54"/>
-      <c r="E69" s="54"/>
-      <c r="F69" s="54"/>
-      <c r="G69" s="54"/>
-      <c r="H69" s="54"/>
-      <c r="I69" s="54"/>
+      <c r="B69" s="56"/>
+      <c r="C69" s="56"/>
+      <c r="D69" s="56"/>
+      <c r="E69" s="56"/>
+      <c r="F69" s="56"/>
+      <c r="G69" s="56"/>
+      <c r="H69" s="56"/>
+      <c r="I69" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
-      <c r="B70" s="54"/>
-      <c r="C70" s="54"/>
-      <c r="D70" s="54"/>
-      <c r="E70" s="54"/>
-      <c r="F70" s="54"/>
-      <c r="G70" s="54"/>
-      <c r="H70" s="54"/>
-      <c r="I70" s="54"/>
+      <c r="B70" s="56"/>
+      <c r="C70" s="56"/>
+      <c r="D70" s="56"/>
+      <c r="E70" s="56"/>
+      <c r="F70" s="56"/>
+      <c r="G70" s="56"/>
+      <c r="H70" s="56"/>
+      <c r="I70" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
-      <c r="B71" s="54"/>
-      <c r="C71" s="54"/>
-      <c r="D71" s="54"/>
-      <c r="E71" s="54"/>
-      <c r="F71" s="54"/>
-      <c r="G71" s="54"/>
-      <c r="H71" s="54"/>
-      <c r="I71" s="54"/>
+      <c r="B71" s="56"/>
+      <c r="C71" s="56"/>
+      <c r="D71" s="56"/>
+      <c r="E71" s="56"/>
+      <c r="F71" s="56"/>
+      <c r="G71" s="56"/>
+      <c r="H71" s="56"/>
+      <c r="I71" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
-      <c r="B72" s="54"/>
-      <c r="C72" s="54"/>
-      <c r="D72" s="54"/>
-      <c r="E72" s="54"/>
-      <c r="F72" s="54"/>
-      <c r="G72" s="54"/>
-      <c r="H72" s="54"/>
-      <c r="I72" s="54"/>
+      <c r="B72" s="56"/>
+      <c r="C72" s="56"/>
+      <c r="D72" s="56"/>
+      <c r="E72" s="56"/>
+      <c r="F72" s="56"/>
+      <c r="G72" s="56"/>
+      <c r="H72" s="56"/>
+      <c r="I72" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="73">
-      <c r="B73" s="54"/>
-      <c r="C73" s="54"/>
-      <c r="D73" s="54"/>
-      <c r="E73" s="54"/>
-      <c r="F73" s="54"/>
-      <c r="G73" s="54"/>
-      <c r="H73" s="54"/>
-      <c r="I73" s="54"/>
+      <c r="B73" s="56"/>
+      <c r="C73" s="56"/>
+      <c r="D73" s="56"/>
+      <c r="E73" s="56"/>
+      <c r="F73" s="56"/>
+      <c r="G73" s="56"/>
+      <c r="H73" s="56"/>
+      <c r="I73" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="74">
-      <c r="B74" s="54"/>
-      <c r="C74" s="54"/>
-      <c r="D74" s="54"/>
-      <c r="E74" s="54"/>
-      <c r="F74" s="54"/>
-      <c r="G74" s="54"/>
-      <c r="H74" s="54"/>
-      <c r="I74" s="54"/>
+      <c r="B74" s="56"/>
+      <c r="C74" s="56"/>
+      <c r="D74" s="56"/>
+      <c r="E74" s="56"/>
+      <c r="F74" s="56"/>
+      <c r="G74" s="56"/>
+      <c r="H74" s="56"/>
+      <c r="I74" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="75">
-      <c r="B75" s="54"/>
-      <c r="C75" s="54"/>
-      <c r="D75" s="54"/>
-      <c r="E75" s="54"/>
-      <c r="F75" s="54"/>
-      <c r="G75" s="54"/>
-      <c r="H75" s="54"/>
-      <c r="I75" s="54"/>
+      <c r="B75" s="56"/>
+      <c r="C75" s="56"/>
+      <c r="D75" s="56"/>
+      <c r="E75" s="56"/>
+      <c r="F75" s="56"/>
+      <c r="G75" s="56"/>
+      <c r="H75" s="56"/>
+      <c r="I75" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="76">
-      <c r="B76" s="54"/>
-      <c r="C76" s="54"/>
-      <c r="D76" s="54"/>
-      <c r="E76" s="54"/>
-      <c r="F76" s="54"/>
-      <c r="G76" s="54"/>
-      <c r="H76" s="54"/>
-      <c r="I76" s="54"/>
+      <c r="B76" s="56"/>
+      <c r="C76" s="56"/>
+      <c r="D76" s="56"/>
+      <c r="E76" s="56"/>
+      <c r="F76" s="56"/>
+      <c r="G76" s="56"/>
+      <c r="H76" s="56"/>
+      <c r="I76" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="77">
-      <c r="B77" s="54"/>
-      <c r="C77" s="54"/>
-      <c r="D77" s="54"/>
-      <c r="E77" s="54"/>
-      <c r="F77" s="54"/>
-      <c r="G77" s="54"/>
-      <c r="H77" s="54"/>
-      <c r="I77" s="54"/>
+      <c r="B77" s="56"/>
+      <c r="C77" s="56"/>
+      <c r="D77" s="56"/>
+      <c r="E77" s="56"/>
+      <c r="F77" s="56"/>
+      <c r="G77" s="56"/>
+      <c r="H77" s="56"/>
+      <c r="I77" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="78">
-      <c r="B78" s="54"/>
-      <c r="C78" s="54"/>
-      <c r="D78" s="54"/>
-      <c r="E78" s="54"/>
-      <c r="F78" s="54"/>
-      <c r="G78" s="54"/>
-      <c r="H78" s="54"/>
-      <c r="I78" s="54"/>
+      <c r="B78" s="56"/>
+      <c r="C78" s="56"/>
+      <c r="D78" s="56"/>
+      <c r="E78" s="56"/>
+      <c r="F78" s="56"/>
+      <c r="G78" s="56"/>
+      <c r="H78" s="56"/>
+      <c r="I78" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="79">
-      <c r="B79" s="54"/>
-      <c r="C79" s="54"/>
-      <c r="D79" s="54"/>
-      <c r="E79" s="54"/>
-      <c r="F79" s="54"/>
-      <c r="G79" s="54"/>
-      <c r="H79" s="54"/>
-      <c r="I79" s="54"/>
+      <c r="B79" s="56"/>
+      <c r="C79" s="56"/>
+      <c r="D79" s="56"/>
+      <c r="E79" s="56"/>
+      <c r="F79" s="56"/>
+      <c r="G79" s="56"/>
+      <c r="H79" s="56"/>
+      <c r="I79" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="80">
-      <c r="B80" s="54"/>
-      <c r="C80" s="54"/>
-      <c r="D80" s="54"/>
-      <c r="E80" s="54"/>
-      <c r="F80" s="54"/>
-      <c r="G80" s="54"/>
-      <c r="H80" s="54"/>
-      <c r="I80" s="54"/>
+      <c r="B80" s="56"/>
+      <c r="C80" s="56"/>
+      <c r="D80" s="56"/>
+      <c r="E80" s="56"/>
+      <c r="F80" s="56"/>
+      <c r="G80" s="56"/>
+      <c r="H80" s="56"/>
+      <c r="I80" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="81">
-      <c r="B81" s="54"/>
-      <c r="C81" s="54"/>
-      <c r="D81" s="54"/>
-      <c r="E81" s="54"/>
-      <c r="F81" s="54"/>
-      <c r="G81" s="54"/>
-      <c r="H81" s="54"/>
-      <c r="I81" s="54"/>
+      <c r="B81" s="56"/>
+      <c r="C81" s="56"/>
+      <c r="D81" s="56"/>
+      <c r="E81" s="56"/>
+      <c r="F81" s="56"/>
+      <c r="G81" s="56"/>
+      <c r="H81" s="56"/>
+      <c r="I81" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="82">
-      <c r="B82" s="54"/>
-      <c r="C82" s="54"/>
-      <c r="D82" s="54"/>
-      <c r="E82" s="54"/>
-      <c r="F82" s="54"/>
-      <c r="G82" s="54"/>
-      <c r="H82" s="54"/>
-      <c r="I82" s="54"/>
+      <c r="B82" s="56"/>
+      <c r="C82" s="56"/>
+      <c r="D82" s="56"/>
+      <c r="E82" s="56"/>
+      <c r="F82" s="56"/>
+      <c r="G82" s="56"/>
+      <c r="H82" s="56"/>
+      <c r="I82" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="83">
-      <c r="B83" s="54"/>
-      <c r="C83" s="54"/>
-      <c r="D83" s="54"/>
-      <c r="E83" s="54"/>
-      <c r="F83" s="54"/>
-      <c r="G83" s="54"/>
-      <c r="H83" s="54"/>
-      <c r="I83" s="54"/>
+      <c r="B83" s="56"/>
+      <c r="C83" s="56"/>
+      <c r="D83" s="56"/>
+      <c r="E83" s="56"/>
+      <c r="F83" s="56"/>
+      <c r="G83" s="56"/>
+      <c r="H83" s="56"/>
+      <c r="I83" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="84">
-      <c r="B84" s="54"/>
-      <c r="C84" s="54"/>
-      <c r="D84" s="54"/>
-      <c r="E84" s="54"/>
-      <c r="F84" s="54"/>
-      <c r="G84" s="54"/>
-      <c r="H84" s="54"/>
-      <c r="I84" s="54"/>
+      <c r="B84" s="56"/>
+      <c r="C84" s="56"/>
+      <c r="D84" s="56"/>
+      <c r="E84" s="56"/>
+      <c r="F84" s="56"/>
+      <c r="G84" s="56"/>
+      <c r="H84" s="56"/>
+      <c r="I84" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="85">
-      <c r="B85" s="54"/>
-      <c r="C85" s="54"/>
-      <c r="D85" s="54"/>
-      <c r="E85" s="54"/>
-      <c r="F85" s="54"/>
-      <c r="G85" s="54"/>
-      <c r="H85" s="54"/>
-      <c r="I85" s="54"/>
+      <c r="B85" s="56"/>
+      <c r="C85" s="56"/>
+      <c r="D85" s="56"/>
+      <c r="E85" s="56"/>
+      <c r="F85" s="56"/>
+      <c r="G85" s="56"/>
+      <c r="H85" s="56"/>
+      <c r="I85" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="86">
-      <c r="B86" s="54"/>
-      <c r="C86" s="54"/>
-      <c r="D86" s="54"/>
-      <c r="E86" s="54"/>
-      <c r="F86" s="54"/>
-      <c r="G86" s="54"/>
-      <c r="H86" s="54"/>
-      <c r="I86" s="54"/>
+      <c r="B86" s="56"/>
+      <c r="C86" s="56"/>
+      <c r="D86" s="56"/>
+      <c r="E86" s="56"/>
+      <c r="F86" s="56"/>
+      <c r="G86" s="56"/>
+      <c r="H86" s="56"/>
+      <c r="I86" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87">
-      <c r="B87" s="54"/>
-      <c r="C87" s="54"/>
-      <c r="D87" s="54"/>
-      <c r="E87" s="54"/>
-      <c r="F87" s="54"/>
-      <c r="G87" s="54"/>
-      <c r="H87" s="54"/>
-      <c r="I87" s="54"/>
+      <c r="B87" s="56"/>
+      <c r="C87" s="56"/>
+      <c r="D87" s="56"/>
+      <c r="E87" s="56"/>
+      <c r="F87" s="56"/>
+      <c r="G87" s="56"/>
+      <c r="H87" s="56"/>
+      <c r="I87" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="88">
-      <c r="B88" s="54"/>
-      <c r="C88" s="54"/>
-      <c r="D88" s="54"/>
-      <c r="E88" s="54"/>
-      <c r="F88" s="54"/>
-      <c r="G88" s="54"/>
-      <c r="H88" s="54"/>
-      <c r="I88" s="54"/>
+      <c r="B88" s="56"/>
+      <c r="C88" s="56"/>
+      <c r="D88" s="56"/>
+      <c r="E88" s="56"/>
+      <c r="F88" s="56"/>
+      <c r="G88" s="56"/>
+      <c r="H88" s="56"/>
+      <c r="I88" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="89">
-      <c r="B89" s="54"/>
-      <c r="C89" s="54"/>
-      <c r="D89" s="54"/>
-      <c r="E89" s="54"/>
-      <c r="F89" s="54"/>
-      <c r="G89" s="54"/>
-      <c r="H89" s="54"/>
-      <c r="I89" s="54"/>
+      <c r="B89" s="56"/>
+      <c r="C89" s="56"/>
+      <c r="D89" s="56"/>
+      <c r="E89" s="56"/>
+      <c r="F89" s="56"/>
+      <c r="G89" s="56"/>
+      <c r="H89" s="56"/>
+      <c r="I89" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="90">
-      <c r="B90" s="54"/>
-      <c r="C90" s="54"/>
-      <c r="D90" s="54"/>
-      <c r="E90" s="54"/>
-      <c r="F90" s="54"/>
-      <c r="G90" s="54"/>
-      <c r="H90" s="54"/>
-      <c r="I90" s="54"/>
+      <c r="B90" s="56"/>
+      <c r="C90" s="56"/>
+      <c r="D90" s="56"/>
+      <c r="E90" s="56"/>
+      <c r="F90" s="56"/>
+      <c r="G90" s="56"/>
+      <c r="H90" s="56"/>
+      <c r="I90" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="91">
-      <c r="B91" s="54"/>
-      <c r="C91" s="54"/>
-      <c r="D91" s="54"/>
-      <c r="E91" s="54"/>
-      <c r="F91" s="54"/>
-      <c r="G91" s="54"/>
-      <c r="H91" s="54"/>
-      <c r="I91" s="54"/>
+      <c r="B91" s="56"/>
+      <c r="C91" s="56"/>
+      <c r="D91" s="56"/>
+      <c r="E91" s="56"/>
+      <c r="F91" s="56"/>
+      <c r="G91" s="56"/>
+      <c r="H91" s="56"/>
+      <c r="I91" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
-      <c r="B92" s="54"/>
-      <c r="C92" s="54"/>
-      <c r="D92" s="54"/>
-      <c r="E92" s="54"/>
-      <c r="F92" s="54"/>
-      <c r="G92" s="54"/>
-      <c r="H92" s="54"/>
-      <c r="I92" s="54"/>
+      <c r="B92" s="56"/>
+      <c r="C92" s="56"/>
+      <c r="D92" s="56"/>
+      <c r="E92" s="56"/>
+      <c r="F92" s="56"/>
+      <c r="G92" s="56"/>
+      <c r="H92" s="56"/>
+      <c r="I92" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93">
-      <c r="B93" s="54"/>
-      <c r="C93" s="54"/>
-      <c r="D93" s="54"/>
-      <c r="E93" s="54"/>
-      <c r="F93" s="54"/>
-      <c r="G93" s="54"/>
-      <c r="H93" s="54"/>
-      <c r="I93" s="54"/>
+      <c r="B93" s="56"/>
+      <c r="C93" s="56"/>
+      <c r="D93" s="56"/>
+      <c r="E93" s="56"/>
+      <c r="F93" s="56"/>
+      <c r="G93" s="56"/>
+      <c r="H93" s="56"/>
+      <c r="I93" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="94">
-      <c r="B94" s="54"/>
-      <c r="C94" s="54"/>
-      <c r="D94" s="54"/>
-      <c r="E94" s="54"/>
-      <c r="F94" s="54"/>
-      <c r="G94" s="54"/>
-      <c r="H94" s="54"/>
-      <c r="I94" s="54"/>
+      <c r="B94" s="56"/>
+      <c r="C94" s="56"/>
+      <c r="D94" s="56"/>
+      <c r="E94" s="56"/>
+      <c r="F94" s="56"/>
+      <c r="G94" s="56"/>
+      <c r="H94" s="56"/>
+      <c r="I94" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="95">
-      <c r="B95" s="54"/>
-      <c r="C95" s="54"/>
-      <c r="D95" s="54"/>
-      <c r="E95" s="54"/>
-      <c r="F95" s="54"/>
-      <c r="G95" s="54"/>
-      <c r="H95" s="54"/>
-      <c r="I95" s="54"/>
+      <c r="B95" s="56"/>
+      <c r="C95" s="56"/>
+      <c r="D95" s="56"/>
+      <c r="E95" s="56"/>
+      <c r="F95" s="56"/>
+      <c r="G95" s="56"/>
+      <c r="H95" s="56"/>
+      <c r="I95" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="96">
-      <c r="B96" s="54"/>
-      <c r="C96" s="54"/>
-      <c r="D96" s="54"/>
-      <c r="E96" s="54"/>
-      <c r="F96" s="54"/>
-      <c r="G96" s="54"/>
-      <c r="H96" s="54"/>
-      <c r="I96" s="54"/>
+      <c r="B96" s="56"/>
+      <c r="C96" s="56"/>
+      <c r="D96" s="56"/>
+      <c r="E96" s="56"/>
+      <c r="F96" s="56"/>
+      <c r="G96" s="56"/>
+      <c r="H96" s="56"/>
+      <c r="I96" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="97">
-      <c r="B97" s="54"/>
-      <c r="C97" s="54"/>
-      <c r="D97" s="54"/>
-      <c r="E97" s="54"/>
-      <c r="F97" s="54"/>
-      <c r="G97" s="54"/>
-      <c r="H97" s="54"/>
-      <c r="I97" s="54"/>
+      <c r="B97" s="56"/>
+      <c r="C97" s="56"/>
+      <c r="D97" s="56"/>
+      <c r="E97" s="56"/>
+      <c r="F97" s="56"/>
+      <c r="G97" s="56"/>
+      <c r="H97" s="56"/>
+      <c r="I97" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="98">
-      <c r="B98" s="54"/>
-      <c r="C98" s="54"/>
-      <c r="D98" s="54"/>
-      <c r="E98" s="54"/>
-      <c r="F98" s="54"/>
-      <c r="G98" s="54"/>
-      <c r="H98" s="54"/>
-      <c r="I98" s="54"/>
+      <c r="B98" s="56"/>
+      <c r="C98" s="56"/>
+      <c r="D98" s="56"/>
+      <c r="E98" s="56"/>
+      <c r="F98" s="56"/>
+      <c r="G98" s="56"/>
+      <c r="H98" s="56"/>
+      <c r="I98" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="99">
-      <c r="B99" s="54"/>
-      <c r="C99" s="54"/>
-      <c r="D99" s="54"/>
-      <c r="E99" s="54"/>
-      <c r="F99" s="54"/>
-      <c r="G99" s="54"/>
-      <c r="H99" s="54"/>
-      <c r="I99" s="54"/>
+      <c r="B99" s="56"/>
+      <c r="C99" s="56"/>
+      <c r="D99" s="56"/>
+      <c r="E99" s="56"/>
+      <c r="F99" s="56"/>
+      <c r="G99" s="56"/>
+      <c r="H99" s="56"/>
+      <c r="I99" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">
-      <c r="B100" s="54"/>
-      <c r="C100" s="54"/>
-      <c r="D100" s="54"/>
-      <c r="E100" s="54"/>
-      <c r="F100" s="54"/>
-      <c r="G100" s="54"/>
-      <c r="H100" s="54"/>
-      <c r="I100" s="54"/>
+      <c r="B100" s="56"/>
+      <c r="C100" s="56"/>
+      <c r="D100" s="56"/>
+      <c r="E100" s="56"/>
+      <c r="F100" s="56"/>
+      <c r="G100" s="56"/>
+      <c r="H100" s="56"/>
+      <c r="I100" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="101">
-      <c r="B101" s="54"/>
-      <c r="C101" s="54"/>
-      <c r="D101" s="54"/>
-      <c r="E101" s="54"/>
-      <c r="F101" s="54"/>
-      <c r="G101" s="54"/>
-      <c r="H101" s="54"/>
-      <c r="I101" s="54"/>
+      <c r="B101" s="56"/>
+      <c r="C101" s="56"/>
+      <c r="D101" s="56"/>
+      <c r="E101" s="56"/>
+      <c r="F101" s="56"/>
+      <c r="G101" s="56"/>
+      <c r="H101" s="56"/>
+      <c r="I101" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="102">
-      <c r="B102" s="54"/>
-      <c r="C102" s="54"/>
-      <c r="D102" s="54"/>
-      <c r="E102" s="54"/>
-      <c r="F102" s="54"/>
-      <c r="G102" s="54"/>
-      <c r="H102" s="54"/>
-      <c r="I102" s="54"/>
+      <c r="B102" s="56"/>
+      <c r="C102" s="56"/>
+      <c r="D102" s="56"/>
+      <c r="E102" s="56"/>
+      <c r="F102" s="56"/>
+      <c r="G102" s="56"/>
+      <c r="H102" s="56"/>
+      <c r="I102" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="103">
-      <c r="B103" s="54"/>
-      <c r="C103" s="54"/>
-      <c r="D103" s="54"/>
-      <c r="E103" s="54"/>
-      <c r="F103" s="54"/>
-      <c r="G103" s="54"/>
-      <c r="H103" s="54"/>
-      <c r="I103" s="54"/>
+      <c r="B103" s="56"/>
+      <c r="C103" s="56"/>
+      <c r="D103" s="56"/>
+      <c r="E103" s="56"/>
+      <c r="F103" s="56"/>
+      <c r="G103" s="56"/>
+      <c r="H103" s="56"/>
+      <c r="I103" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="104">
-      <c r="B104" s="54"/>
-      <c r="C104" s="54"/>
-      <c r="D104" s="54"/>
-      <c r="E104" s="54"/>
-      <c r="F104" s="54"/>
-      <c r="G104" s="54"/>
-      <c r="H104" s="54"/>
-      <c r="I104" s="54"/>
+      <c r="B104" s="56"/>
+      <c r="C104" s="56"/>
+      <c r="D104" s="56"/>
+      <c r="E104" s="56"/>
+      <c r="F104" s="56"/>
+      <c r="G104" s="56"/>
+      <c r="H104" s="56"/>
+      <c r="I104" s="56"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="105">
-      <c r="B105" s="54"/>
-      <c r="C105" s="54"/>
-      <c r="D105" s="54"/>
-      <c r="E105" s="54"/>
-      <c r="F105" s="54"/>
-      <c r="G105" s="54"/>
-      <c r="H105" s="54"/>
-      <c r="I105" s="54"/>
+      <c r="B105" s="56"/>
+      <c r="C105" s="56"/>
+      <c r="D105" s="56"/>
+      <c r="E105" s="56"/>
+      <c r="F105" s="56"/>
+      <c r="G105" s="56"/>
+      <c r="H105" s="56"/>
+      <c r="I105" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2012,18 +2018,18 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9019607843137"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.5960784313725"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.556862745098"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.9843137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.6078431372549"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.2392156862745"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="35.843137254902"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.7176470588235"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="41.043137254902"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.9019607843137"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.678431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.9019607843137"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9647058823529"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.8313725490196"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7098039215686"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.1921568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7254901960784"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.4352941176471"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0235294117647"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.8509803921569"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="41.243137254902"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.9647058823529"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.7529411764706"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.9647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
@@ -2032,154 +2038,154 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="63" t="s">
+      <c r="B5" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="63" t="s">
+      <c r="D5" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="63" t="s">
+      <c r="E5" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="63" t="s">
+      <c r="F5" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="G5" s="63" t="s">
+      <c r="G5" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="H5" s="63" t="s">
+      <c r="H5" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="63" t="s">
+      <c r="I5" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="K5" s="63"/>
-      <c r="L5" s="63"/>
-      <c r="M5" s="63"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="65" t="s">
         <v>79</v>
       </c>
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="63" t="s">
+      <c r="E6" s="65" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="63" t="s">
+      <c r="F6" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="G6" s="63" t="s">
+      <c r="G6" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="63" t="s">
+      <c r="H6" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="63" t="s">
+      <c r="I6" s="65" t="s">
         <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="C7" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="66" t="s">
         <v>89</v>
       </c>
-      <c r="E7" s="66" t="s">
+      <c r="E7" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="65" t="s">
+      <c r="F7" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="65" t="s">
+      <c r="G7" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="H7" s="65" t="s">
+      <c r="H7" s="67" t="s">
         <v>92</v>
       </c>
-      <c r="I7" s="67" t="s">
+      <c r="I7" s="69" t="s">
         <v>93</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
-      <c r="B8" s="64" t="s">
+      <c r="B8" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="67" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="64" t="s">
+      <c r="D8" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="64" t="s">
+      <c r="E8" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="F8" s="64" t="s">
+      <c r="F8" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="H8" s="65" t="s">
+      <c r="H8" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="I8" s="67" t="s">
+      <c r="I8" s="69" t="s">
         <v>100</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
-      <c r="B9" s="64" t="s">
+      <c r="B9" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="66" t="s">
+      <c r="E9" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="66" t="s">
         <v>105</v>
       </c>
-      <c r="I9" s="67" t="s">
+      <c r="I9" s="69" t="s">
         <v>106</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="67" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="67" t="s">
         <v>107</v>
       </c>
-      <c r="I10" s="67" t="s">
+      <c r="I10" s="69" t="s">
         <v>108</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="67" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="C11" s="67" t="s">
         <v>110</v>
       </c>
-      <c r="I11" s="68" t="s">
+      <c r="I11" s="70" t="s">
         <v>111</v>
       </c>
       <c r="J11" s="0" t="n">
@@ -2187,13 +2193,13 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C12" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="I12" s="68" t="s">
+      <c r="I12" s="70" t="s">
         <v>114</v>
       </c>
       <c r="J12" s="0" t="n">
@@ -2201,33 +2207,33 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
-      <c r="B13" s="65" t="s">
+      <c r="B13" s="67" t="s">
         <v>115</v>
       </c>
-      <c r="I13" s="68" t="s">
+      <c r="I13" s="70" t="s">
         <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="B14" s="65" t="s">
+      <c r="B14" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="I14" s="68" t="s">
+      <c r="I14" s="70" t="s">
         <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="67" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
-      <c r="B19" s="64" t="s">
+      <c r="B19" s="66" t="s">
         <v>72</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
-      <c r="B20" s="66" t="s">
+      <c r="B20" s="68" t="s">
         <v>119</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Organizacion de documentos acorde a nombre
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Configuracion/PlanConfiguracion.xlsx
+++ b/qualtcom/Organizacional/Configuracion/PlanConfiguracion.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="122">
   <si>
     <t>Plan de Administración de Configuración</t>
   </si>
@@ -90,94 +90,100 @@
     <t>Plan_calidad</t>
   </si>
   <si>
+    <t>Checklist Procesos</t>
+  </si>
+  <si>
+    <t>PTL_Checklist_procesos</t>
+  </si>
+  <si>
+    <t>Checklist Organizacional</t>
+  </si>
+  <si>
+    <t>Checklist_Organizacional_YYMMDD</t>
+  </si>
+  <si>
+    <t>Políticas</t>
+  </si>
+  <si>
+    <t>Políticas Soporte</t>
+  </si>
+  <si>
+    <t>Políticas de soporte</t>
+  </si>
+  <si>
+    <t>Políticas Organizacionales</t>
+  </si>
+  <si>
+    <t>Políticas_organizacionales</t>
+  </si>
+  <si>
+    <t>Planeación</t>
+  </si>
+  <si>
+    <t>Plan de Riesgos</t>
+  </si>
+  <si>
+    <t>PTL_Plan_riesgos</t>
+  </si>
+  <si>
+    <t>Estimación</t>
+  </si>
+  <si>
+    <t>PTL_Estimación</t>
+  </si>
+  <si>
+    <t>Plan Estratégico</t>
+  </si>
+  <si>
+    <t>PTL_Plan_estratégico</t>
+  </si>
+  <si>
+    <t>Cambios</t>
+  </si>
+  <si>
+    <t>Solicitud de cambios</t>
+  </si>
+  <si>
+    <t>PTL_Solicitud Cambios</t>
+  </si>
+  <si>
+    <t>Procesos</t>
+  </si>
+  <si>
+    <t>Línea Base</t>
+  </si>
+  <si>
+    <t>Plan_riesgos</t>
+  </si>
+  <si>
+    <t>Plan_estratégico</t>
+  </si>
+  <si>
+    <t>Minuta de compromiso</t>
+  </si>
+  <si>
+    <t>Minuta_compromiso</t>
+  </si>
+  <si>
+    <t>Catalogo de servicios</t>
+  </si>
+  <si>
+    <t>Catalogo_servicios</t>
+  </si>
+  <si>
+    <t>Solicitud_Cambios_YYMMDD</t>
+  </si>
+  <si>
     <t>Checklist Auditoría</t>
   </si>
   <si>
-    <t>PTL_Checklist_Auditoría</t>
-  </si>
-  <si>
-    <t>Auditoría Organizacional</t>
-  </si>
-  <si>
-    <t>Auditoría_Organizacional_YYMMDD</t>
-  </si>
-  <si>
-    <t>Políticas</t>
-  </si>
-  <si>
-    <t>Políticas Soporte</t>
-  </si>
-  <si>
-    <t>Políticas de soporte</t>
-  </si>
-  <si>
-    <t>Políticas Organizacionales</t>
-  </si>
-  <si>
-    <t>Políticas_organizacionales</t>
-  </si>
-  <si>
-    <t>Planeación</t>
-  </si>
-  <si>
-    <t>Plan de Riesgos</t>
-  </si>
-  <si>
-    <t>PTL_Plan_riesgos</t>
-  </si>
-  <si>
-    <t>Estimación</t>
-  </si>
-  <si>
-    <t>PTL_Estimación</t>
-  </si>
-  <si>
-    <t>Plan Estratégico</t>
-  </si>
-  <si>
-    <t>PTL_Plan_estratégico</t>
-  </si>
-  <si>
-    <t>Catalogo de servicios</t>
-  </si>
-  <si>
-    <t>PTL_Catalogo_servicios</t>
-  </si>
-  <si>
-    <t>Cambios</t>
-  </si>
-  <si>
-    <t>Solicitud de cambios</t>
-  </si>
-  <si>
-    <t>PTL_Solicitud Cambios</t>
-  </si>
-  <si>
-    <t>Procesos</t>
-  </si>
-  <si>
-    <t>Línea Base</t>
-  </si>
-  <si>
-    <t>Plan_riesgos</t>
-  </si>
-  <si>
-    <t>Plan_estratégico</t>
-  </si>
-  <si>
-    <t>Minuta de compromiso</t>
-  </si>
-  <si>
-    <t>Minuta_compromiso</t>
-  </si>
-  <si>
-    <t>Catalogo_servicios</t>
-  </si>
-  <si>
-    <t>Solicitud_Cambios_YYMMDD</t>
-  </si>
-  <si>
     <t>Checklist_Auditoría_YYMMDD</t>
+  </si>
+  <si>
+    <t>Pólizas</t>
+  </si>
+  <si>
+    <t>Encuestas de satisfacción</t>
   </si>
   <si>
     <t>Linea Base</t>
@@ -554,7 +560,7 @@
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -576,13 +582,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00B3B3B3"/>
-        <bgColor rgb="00CCCCCC"/>
+        <bgColor rgb="00C0C0C0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00CCCCCC"/>
-        <bgColor rgb="00CFE7F5"/>
+        <bgColor rgb="00C0C0C0"/>
       </patternFill>
     </fill>
     <fill>
@@ -595,6 +601,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00999999"/>
         <bgColor rgb="00808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C0C0C0"/>
+        <bgColor rgb="00CCCCCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -753,7 +765,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
@@ -792,11 +804,14 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="4" fontId="8" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="8" fontId="12" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="8" fontId="8" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="8" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="8" fontId="8" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="9" fontId="12" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="9" fontId="8" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="9" fontId="8" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="6" fontId="11" numFmtId="164" xfId="0"/>
@@ -815,6 +830,9 @@
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="4" fontId="13" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="8" fontId="11" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="6" fontId="11" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
@@ -899,11 +917,11 @@
       <alignment horizontal="left" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="21" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="9" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="10" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="11" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="12" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="10" fontId="21" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="13" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="11" fontId="21" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -929,7 +947,7 @@
       <rgbColor rgb="00808000"/>
       <rgbColor rgb="00800080"/>
       <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00CCCCCC"/>
+      <rgbColor rgb="00C0C0C0"/>
       <rgbColor rgb="00808080"/>
       <rgbColor rgb="009999FF"/>
       <rgbColor rgb="00993366"/>
@@ -938,7 +956,7 @@
       <rgbColor rgb="00660066"/>
       <rgbColor rgb="00FF8080"/>
       <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00B3B3B3"/>
+      <rgbColor rgb="00CCCCCC"/>
       <rgbColor rgb="00000080"/>
       <rgbColor rgb="00FF00FF"/>
       <rgbColor rgb="00FFFF00"/>
@@ -953,7 +971,7 @@
       <rgbColor rgb="00FFFF99"/>
       <rgbColor rgb="0089C3E5"/>
       <rgbColor rgb="00E69CA4"/>
-      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00B3B3B3"/>
       <rgbColor rgb="00FFCC99"/>
       <rgbColor rgb="003366FF"/>
       <rgbColor rgb="0033CCCC"/>
@@ -981,57 +999,57 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A32" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C36" activeCellId="0" pane="topLeft" sqref="C36"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A5" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C10" activeCellId="0" pane="topLeft" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="2.80392156862745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="50.7843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.5764705882353"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="68.0941176470588"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.4862745098039"/>
-    <col collapsed="false" hidden="false" max="251" min="6" style="1" width="11.9647058823529"/>
-    <col collapsed="false" hidden="false" max="252" min="252" style="1" width="2.80392156862745"/>
-    <col collapsed="false" hidden="false" max="253" min="253" style="1" width="48.2156862745098"/>
-    <col collapsed="false" hidden="false" max="254" min="254" style="1" width="60.4156862745098"/>
-    <col collapsed="false" hidden="false" max="255" min="255" style="1" width="31.8274509803922"/>
-    <col collapsed="false" hidden="false" max="256" min="256" style="1" width="11.4862745098039"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="2.82352941176471"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.0352941176471"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.8196078431373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="68.4313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.6039215686274"/>
+    <col collapsed="false" hidden="false" max="251" min="6" style="1" width="12.0196078431373"/>
+    <col collapsed="false" hidden="false" max="252" min="252" style="1" width="2.82352941176471"/>
+    <col collapsed="false" hidden="false" max="253" min="253" style="1" width="48.4509803921569"/>
+    <col collapsed="false" hidden="false" max="254" min="254" style="1" width="60.7137254901961"/>
+    <col collapsed="false" hidden="false" max="255" min="255" style="1" width="31.9882352941176"/>
+    <col collapsed="false" hidden="false" max="256" min="256" style="1" width="11.5411764705882"/>
     <col collapsed="false" hidden="false" max="257" min="257" style="1" width="1.12941176470588"/>
-    <col collapsed="false" hidden="false" max="258" min="258" style="1" width="28.3372549019608"/>
-    <col collapsed="false" hidden="false" max="259" min="259" style="1" width="23.4862745098039"/>
-    <col collapsed="false" hidden="false" max="260" min="260" style="1" width="2.42352941176471"/>
-    <col collapsed="false" hidden="false" max="261" min="261" style="1" width="23.4862745098039"/>
-    <col collapsed="false" hidden="false" max="507" min="262" style="1" width="11.9647058823529"/>
-    <col collapsed="false" hidden="false" max="508" min="508" style="1" width="2.80392156862745"/>
-    <col collapsed="false" hidden="false" max="509" min="509" style="1" width="48.2156862745098"/>
-    <col collapsed="false" hidden="false" max="510" min="510" style="1" width="60.4156862745098"/>
-    <col collapsed="false" hidden="false" max="511" min="511" style="1" width="31.8274509803922"/>
-    <col collapsed="false" hidden="false" max="512" min="512" style="1" width="11.4862745098039"/>
+    <col collapsed="false" hidden="false" max="258" min="258" style="1" width="28.4823529411765"/>
+    <col collapsed="false" hidden="false" max="259" min="259" style="1" width="23.6039215686274"/>
+    <col collapsed="false" hidden="false" max="260" min="260" style="1" width="2.43137254901961"/>
+    <col collapsed="false" hidden="false" max="261" min="261" style="1" width="23.6039215686274"/>
+    <col collapsed="false" hidden="false" max="507" min="262" style="1" width="12.0196078431373"/>
+    <col collapsed="false" hidden="false" max="508" min="508" style="1" width="2.82352941176471"/>
+    <col collapsed="false" hidden="false" max="509" min="509" style="1" width="48.4509803921569"/>
+    <col collapsed="false" hidden="false" max="510" min="510" style="1" width="60.7137254901961"/>
+    <col collapsed="false" hidden="false" max="511" min="511" style="1" width="31.9882352941176"/>
+    <col collapsed="false" hidden="false" max="512" min="512" style="1" width="11.5411764705882"/>
     <col collapsed="false" hidden="false" max="513" min="513" style="1" width="1.12941176470588"/>
-    <col collapsed="false" hidden="false" max="514" min="514" style="1" width="28.3372549019608"/>
-    <col collapsed="false" hidden="false" max="515" min="515" style="1" width="23.4862745098039"/>
-    <col collapsed="false" hidden="false" max="516" min="516" style="1" width="2.42352941176471"/>
-    <col collapsed="false" hidden="false" max="517" min="517" style="1" width="23.4862745098039"/>
-    <col collapsed="false" hidden="false" max="763" min="518" style="1" width="11.9647058823529"/>
-    <col collapsed="false" hidden="false" max="764" min="764" style="1" width="2.80392156862745"/>
-    <col collapsed="false" hidden="false" max="765" min="765" style="1" width="48.2156862745098"/>
-    <col collapsed="false" hidden="false" max="766" min="766" style="1" width="60.4156862745098"/>
-    <col collapsed="false" hidden="false" max="767" min="767" style="1" width="31.8274509803922"/>
-    <col collapsed="false" hidden="false" max="768" min="768" style="1" width="11.4862745098039"/>
+    <col collapsed="false" hidden="false" max="514" min="514" style="1" width="28.4823529411765"/>
+    <col collapsed="false" hidden="false" max="515" min="515" style="1" width="23.6039215686274"/>
+    <col collapsed="false" hidden="false" max="516" min="516" style="1" width="2.43137254901961"/>
+    <col collapsed="false" hidden="false" max="517" min="517" style="1" width="23.6039215686274"/>
+    <col collapsed="false" hidden="false" max="763" min="518" style="1" width="12.0196078431373"/>
+    <col collapsed="false" hidden="false" max="764" min="764" style="1" width="2.82352941176471"/>
+    <col collapsed="false" hidden="false" max="765" min="765" style="1" width="48.4509803921569"/>
+    <col collapsed="false" hidden="false" max="766" min="766" style="1" width="60.7137254901961"/>
+    <col collapsed="false" hidden="false" max="767" min="767" style="1" width="31.9882352941176"/>
+    <col collapsed="false" hidden="false" max="768" min="768" style="1" width="11.5411764705882"/>
     <col collapsed="false" hidden="false" max="769" min="769" style="1" width="1.12941176470588"/>
-    <col collapsed="false" hidden="false" max="770" min="770" style="1" width="28.3372549019608"/>
-    <col collapsed="false" hidden="false" max="771" min="771" style="1" width="23.4862745098039"/>
-    <col collapsed="false" hidden="false" max="772" min="772" style="1" width="2.42352941176471"/>
-    <col collapsed="false" hidden="false" max="773" min="773" style="1" width="23.4862745098039"/>
-    <col collapsed="false" hidden="false" max="1019" min="774" style="1" width="11.9647058823529"/>
-    <col collapsed="false" hidden="false" max="1020" min="1020" style="1" width="2.80392156862745"/>
-    <col collapsed="false" hidden="false" max="1021" min="1021" style="1" width="48.2156862745098"/>
-    <col collapsed="false" hidden="false" max="1022" min="1022" style="1" width="60.4156862745098"/>
-    <col collapsed="false" hidden="false" max="1023" min="1023" style="1" width="31.8274509803922"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="11.4862745098039"/>
+    <col collapsed="false" hidden="false" max="770" min="770" style="1" width="28.4823529411765"/>
+    <col collapsed="false" hidden="false" max="771" min="771" style="1" width="23.6039215686274"/>
+    <col collapsed="false" hidden="false" max="772" min="772" style="1" width="2.43137254901961"/>
+    <col collapsed="false" hidden="false" max="773" min="773" style="1" width="23.6039215686274"/>
+    <col collapsed="false" hidden="false" max="1019" min="774" style="1" width="12.0196078431373"/>
+    <col collapsed="false" hidden="false" max="1020" min="1020" style="1" width="2.82352941176471"/>
+    <col collapsed="false" hidden="false" max="1021" min="1021" style="1" width="48.4509803921569"/>
+    <col collapsed="false" hidden="false" max="1022" min="1022" style="1" width="60.7137254901961"/>
+    <col collapsed="false" hidden="false" max="1023" min="1023" style="1" width="31.9882352941176"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="11.5411764705882"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="1">
@@ -1121,7 +1139,7 @@
       <c r="B10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="22" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="15" t="s">
@@ -1166,28 +1184,28 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="14">
       <c r="A14" s="6"/>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="25"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="15">
       <c r="A15" s="6"/>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="27" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="16">
       <c r="A16" s="6"/>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="22" t="s">
         <v>23</v>
       </c>
       <c r="D16" s="15" t="s">
@@ -1196,7 +1214,7 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="17">
       <c r="A17" s="6"/>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="26" t="s">
         <v>24</v>
       </c>
       <c r="C17" s="14" t="s">
@@ -1206,15 +1224,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="18">
       <c r="A18" s="6"/>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="29"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="19">
       <c r="A19" s="6"/>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="26" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="14" t="s">
@@ -1226,10 +1244,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="20">
       <c r="A20" s="6"/>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="22" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="15"/>
@@ -1239,762 +1257,791 @@
       <c r="B21" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="32"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="22">
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="32"/>
+      <c r="D22" s="34"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="23">
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="32"/>
+      <c r="D23" s="34"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="24">
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="32" t="s">
+      <c r="C24" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="D24" s="32"/>
+      <c r="D24" s="34"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="25">
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="32" t="s">
+      <c r="C25" s="36"/>
+      <c r="D25" s="37"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
+      <c r="B26" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="32"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="26">
-      <c r="B26" s="33" t="s">
+      <c r="C26" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="34"/>
-      <c r="D26" s="35"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="27">
-      <c r="B27" s="25" t="s">
+      <c r="D26" s="38"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="27">
+      <c r="A27" s="6"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="28" s="40">
+      <c r="B28" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="29">
+      <c r="B29" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="36"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="16.9" outlineLevel="0" r="28">
-      <c r="A28" s="6"/>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="29" s="38">
-      <c r="B29" s="39" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
+      <c r="B30" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="36"/>
+      <c r="D30" s="37"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
+      <c r="B31" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="30">
-      <c r="B30" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="12" t="s">
+      <c r="D31" s="34"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
+      <c r="B32" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="34"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
+      <c r="B33" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="34"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="34">
+      <c r="B34" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="34"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="35">
+      <c r="B35" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="34"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
+      <c r="B36" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="36"/>
+      <c r="D36" s="37"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="37">
+      <c r="B37" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="38"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
+      <c r="B38" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="36"/>
+      <c r="D38" s="37"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="39">
+      <c r="A39" s="6"/>
+      <c r="B39" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="40">
+      <c r="B40" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="36"/>
+      <c r="D40" s="37"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="41">
+      <c r="A41" s="6"/>
+      <c r="B41" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
+      <c r="B42" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="36"/>
+      <c r="D42" s="37"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="43">
+      <c r="A43" s="6"/>
+      <c r="B43" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="44" s="40">
+      <c r="B44" s="43"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="45">
+      <c r="B45" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="46">
+      <c r="B46" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="D46" s="44" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="47">
+      <c r="B47" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47" s="46"/>
+      <c r="D47" s="47"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="48">
+      <c r="B48" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="C48" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" s="49" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="49">
+      <c r="B49" s="50"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="51"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="50">
+      <c r="A50" s="52"/>
+      <c r="B50" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D30" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="31">
-      <c r="B31" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" s="34"/>
-      <c r="D31" s="35"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="32">
-      <c r="B32" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="32"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="33">
-      <c r="B33" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="32"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="34">
-      <c r="B34" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="32"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="35">
-      <c r="B35" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="C35" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="32"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
-      <c r="B36" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="32"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="37">
-      <c r="B37" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="C37" s="34"/>
-      <c r="D37" s="35"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
-      <c r="B38" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="36"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="39">
-      <c r="B39" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="C39" s="34"/>
-      <c r="D39" s="35"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="40">
-      <c r="A40" s="6"/>
-      <c r="B40" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C40" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="41" s="38">
-      <c r="B41" s="41"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
-      <c r="B42" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="C42" s="39"/>
-      <c r="D42" s="39"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="43">
-      <c r="B43" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="C43" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="D43" s="42" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="44">
-      <c r="B44" s="43" t="s">
-        <v>52</v>
-      </c>
-      <c r="C44" s="44"/>
-      <c r="D44" s="45"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="45">
-      <c r="B45" s="46" t="s">
-        <v>31</v>
-      </c>
-      <c r="C45" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="46">
-      <c r="B46" s="48"/>
-      <c r="C46" s="48"/>
-      <c r="D46" s="49"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="47">
-      <c r="A47" s="50"/>
-      <c r="B47" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" s="9"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="48">
-      <c r="B48" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="C48" s="52"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="49">
-      <c r="B49" s="53" t="s">
-        <v>59</v>
-      </c>
-      <c r="C49" s="54"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="50">
-      <c r="B50" s="55"/>
-      <c r="C50" s="56"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="51">
-      <c r="A51" s="50"/>
-      <c r="B51" s="57" t="s">
+      <c r="C50" s="9"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="51">
+      <c r="B51" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="C51" s="10"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="1" r="52">
-      <c r="B52" s="58" t="s">
+      <c r="C51" s="54"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="52">
+      <c r="B52" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="59"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="1" r="53">
-      <c r="B53" s="60"/>
-      <c r="C53" s="60"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="1" r="54">
-      <c r="B54" s="60"/>
-      <c r="C54" s="60"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="55">
-      <c r="A55" s="56"/>
-      <c r="B55" s="61"/>
-      <c r="C55" s="56"/>
-      <c r="D55" s="56"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="56">
+      <c r="C52" s="56"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
+      <c r="B53" s="57"/>
+      <c r="C53" s="58"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="54">
+      <c r="A54" s="52"/>
+      <c r="B54" s="59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="10"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="1" r="55">
+      <c r="B55" s="60" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="61"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="1" r="56">
       <c r="B56" s="62"/>
-      <c r="C56" s="56"/>
-      <c r="D56" s="56"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="57">
-      <c r="B57" s="56"/>
-      <c r="C57" s="56"/>
-      <c r="D57" s="56"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="58">
-      <c r="A58" s="50"/>
-      <c r="B58" s="57" t="s">
-        <v>62</v>
-      </c>
-      <c r="C58" s="57" t="s">
-        <v>63</v>
-      </c>
-      <c r="D58" s="57" t="s">
+      <c r="C56" s="62"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="1" r="57">
+      <c r="B57" s="62"/>
+      <c r="C57" s="62"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
+      <c r="A58" s="58"/>
+      <c r="B58" s="63"/>
+      <c r="C58" s="58"/>
+      <c r="D58" s="58"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
+      <c r="B59" s="64"/>
+      <c r="C59" s="58"/>
+      <c r="D59" s="58"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
+      <c r="B60" s="58"/>
+      <c r="C60" s="58"/>
+      <c r="D60" s="58"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="61">
+      <c r="A61" s="52"/>
+      <c r="B61" s="59" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
-      <c r="B59" s="63" t="s">
+      <c r="C61" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="C59" s="63" t="s">
+      <c r="D61" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="D59" s="63" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
+      <c r="B62" s="65" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="60">
-      <c r="B60" s="63" t="s">
+      <c r="C62" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="C60" s="63" t="s">
+      <c r="D62" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="D60" s="64" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="63">
+      <c r="B63" s="65" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
-      <c r="B61" s="60"/>
-      <c r="C61" s="60"/>
-      <c r="D61" s="60"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
-      <c r="B62" s="56"/>
-      <c r="C62" s="56"/>
-      <c r="D62" s="56"/>
-      <c r="E62" s="56"/>
-      <c r="F62" s="56"/>
-      <c r="G62" s="56"/>
-      <c r="H62" s="56"/>
-      <c r="I62" s="56"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
-      <c r="B63" s="56"/>
-      <c r="C63" s="56"/>
-      <c r="D63" s="56"/>
-      <c r="E63" s="56"/>
-      <c r="F63" s="56"/>
-      <c r="G63" s="56"/>
-      <c r="H63" s="56"/>
-      <c r="I63" s="56"/>
+      <c r="C63" s="65" t="s">
+        <v>71</v>
+      </c>
+      <c r="D63" s="66" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
-      <c r="B64" s="56"/>
-      <c r="C64" s="56"/>
-      <c r="D64" s="56"/>
-      <c r="E64" s="56"/>
-      <c r="F64" s="56"/>
-      <c r="G64" s="56"/>
-      <c r="H64" s="56"/>
-      <c r="I64" s="56"/>
+      <c r="B64" s="62"/>
+      <c r="C64" s="62"/>
+      <c r="D64" s="62"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
-      <c r="B65" s="56"/>
-      <c r="C65" s="56"/>
-      <c r="D65" s="56"/>
-      <c r="E65" s="56"/>
-      <c r="F65" s="56"/>
-      <c r="G65" s="56"/>
-      <c r="H65" s="56"/>
-      <c r="I65" s="56"/>
+      <c r="B65" s="58"/>
+      <c r="C65" s="58"/>
+      <c r="D65" s="58"/>
+      <c r="E65" s="58"/>
+      <c r="F65" s="58"/>
+      <c r="G65" s="58"/>
+      <c r="H65" s="58"/>
+      <c r="I65" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
-      <c r="B66" s="56"/>
-      <c r="C66" s="56"/>
-      <c r="D66" s="56"/>
-      <c r="E66" s="56"/>
-      <c r="F66" s="56"/>
-      <c r="G66" s="56"/>
-      <c r="H66" s="56"/>
-      <c r="I66" s="56"/>
+      <c r="B66" s="58"/>
+      <c r="C66" s="58"/>
+      <c r="D66" s="58"/>
+      <c r="E66" s="58"/>
+      <c r="F66" s="58"/>
+      <c r="G66" s="58"/>
+      <c r="H66" s="58"/>
+      <c r="I66" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
-      <c r="B67" s="56"/>
-      <c r="C67" s="56"/>
-      <c r="D67" s="56"/>
-      <c r="E67" s="56"/>
-      <c r="F67" s="56"/>
-      <c r="G67" s="56"/>
-      <c r="H67" s="56"/>
-      <c r="I67" s="56"/>
+      <c r="B67" s="58"/>
+      <c r="C67" s="58"/>
+      <c r="D67" s="58"/>
+      <c r="E67" s="58"/>
+      <c r="F67" s="58"/>
+      <c r="G67" s="58"/>
+      <c r="H67" s="58"/>
+      <c r="I67" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
-      <c r="B68" s="56"/>
-      <c r="C68" s="56"/>
-      <c r="D68" s="56"/>
-      <c r="E68" s="56"/>
-      <c r="F68" s="56"/>
-      <c r="G68" s="56"/>
-      <c r="H68" s="56"/>
-      <c r="I68" s="56"/>
+      <c r="B68" s="58"/>
+      <c r="C68" s="58"/>
+      <c r="D68" s="58"/>
+      <c r="E68" s="58"/>
+      <c r="F68" s="58"/>
+      <c r="G68" s="58"/>
+      <c r="H68" s="58"/>
+      <c r="I68" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
-      <c r="B69" s="56"/>
-      <c r="C69" s="56"/>
-      <c r="D69" s="56"/>
-      <c r="E69" s="56"/>
-      <c r="F69" s="56"/>
-      <c r="G69" s="56"/>
-      <c r="H69" s="56"/>
-      <c r="I69" s="56"/>
+      <c r="B69" s="58"/>
+      <c r="C69" s="58"/>
+      <c r="D69" s="58"/>
+      <c r="E69" s="58"/>
+      <c r="F69" s="58"/>
+      <c r="G69" s="58"/>
+      <c r="H69" s="58"/>
+      <c r="I69" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
-      <c r="B70" s="56"/>
-      <c r="C70" s="56"/>
-      <c r="D70" s="56"/>
-      <c r="E70" s="56"/>
-      <c r="F70" s="56"/>
-      <c r="G70" s="56"/>
-      <c r="H70" s="56"/>
-      <c r="I70" s="56"/>
+      <c r="B70" s="58"/>
+      <c r="C70" s="58"/>
+      <c r="D70" s="58"/>
+      <c r="E70" s="58"/>
+      <c r="F70" s="58"/>
+      <c r="G70" s="58"/>
+      <c r="H70" s="58"/>
+      <c r="I70" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
-      <c r="B71" s="56"/>
-      <c r="C71" s="56"/>
-      <c r="D71" s="56"/>
-      <c r="E71" s="56"/>
-      <c r="F71" s="56"/>
-      <c r="G71" s="56"/>
-      <c r="H71" s="56"/>
-      <c r="I71" s="56"/>
+      <c r="B71" s="58"/>
+      <c r="C71" s="58"/>
+      <c r="D71" s="58"/>
+      <c r="E71" s="58"/>
+      <c r="F71" s="58"/>
+      <c r="G71" s="58"/>
+      <c r="H71" s="58"/>
+      <c r="I71" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
-      <c r="B72" s="56"/>
-      <c r="C72" s="56"/>
-      <c r="D72" s="56"/>
-      <c r="E72" s="56"/>
-      <c r="F72" s="56"/>
-      <c r="G72" s="56"/>
-      <c r="H72" s="56"/>
-      <c r="I72" s="56"/>
+      <c r="B72" s="58"/>
+      <c r="C72" s="58"/>
+      <c r="D72" s="58"/>
+      <c r="E72" s="58"/>
+      <c r="F72" s="58"/>
+      <c r="G72" s="58"/>
+      <c r="H72" s="58"/>
+      <c r="I72" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="73">
-      <c r="B73" s="56"/>
-      <c r="C73" s="56"/>
-      <c r="D73" s="56"/>
-      <c r="E73" s="56"/>
-      <c r="F73" s="56"/>
-      <c r="G73" s="56"/>
-      <c r="H73" s="56"/>
-      <c r="I73" s="56"/>
+      <c r="B73" s="58"/>
+      <c r="C73" s="58"/>
+      <c r="D73" s="58"/>
+      <c r="E73" s="58"/>
+      <c r="F73" s="58"/>
+      <c r="G73" s="58"/>
+      <c r="H73" s="58"/>
+      <c r="I73" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="74">
-      <c r="B74" s="56"/>
-      <c r="C74" s="56"/>
-      <c r="D74" s="56"/>
-      <c r="E74" s="56"/>
-      <c r="F74" s="56"/>
-      <c r="G74" s="56"/>
-      <c r="H74" s="56"/>
-      <c r="I74" s="56"/>
+      <c r="B74" s="58"/>
+      <c r="C74" s="58"/>
+      <c r="D74" s="58"/>
+      <c r="E74" s="58"/>
+      <c r="F74" s="58"/>
+      <c r="G74" s="58"/>
+      <c r="H74" s="58"/>
+      <c r="I74" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="75">
-      <c r="B75" s="56"/>
-      <c r="C75" s="56"/>
-      <c r="D75" s="56"/>
-      <c r="E75" s="56"/>
-      <c r="F75" s="56"/>
-      <c r="G75" s="56"/>
-      <c r="H75" s="56"/>
-      <c r="I75" s="56"/>
+      <c r="B75" s="58"/>
+      <c r="C75" s="58"/>
+      <c r="D75" s="58"/>
+      <c r="E75" s="58"/>
+      <c r="F75" s="58"/>
+      <c r="G75" s="58"/>
+      <c r="H75" s="58"/>
+      <c r="I75" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="76">
-      <c r="B76" s="56"/>
-      <c r="C76" s="56"/>
-      <c r="D76" s="56"/>
-      <c r="E76" s="56"/>
-      <c r="F76" s="56"/>
-      <c r="G76" s="56"/>
-      <c r="H76" s="56"/>
-      <c r="I76" s="56"/>
+      <c r="B76" s="58"/>
+      <c r="C76" s="58"/>
+      <c r="D76" s="58"/>
+      <c r="E76" s="58"/>
+      <c r="F76" s="58"/>
+      <c r="G76" s="58"/>
+      <c r="H76" s="58"/>
+      <c r="I76" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="77">
-      <c r="B77" s="56"/>
-      <c r="C77" s="56"/>
-      <c r="D77" s="56"/>
-      <c r="E77" s="56"/>
-      <c r="F77" s="56"/>
-      <c r="G77" s="56"/>
-      <c r="H77" s="56"/>
-      <c r="I77" s="56"/>
+      <c r="B77" s="58"/>
+      <c r="C77" s="58"/>
+      <c r="D77" s="58"/>
+      <c r="E77" s="58"/>
+      <c r="F77" s="58"/>
+      <c r="G77" s="58"/>
+      <c r="H77" s="58"/>
+      <c r="I77" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="78">
-      <c r="B78" s="56"/>
-      <c r="C78" s="56"/>
-      <c r="D78" s="56"/>
-      <c r="E78" s="56"/>
-      <c r="F78" s="56"/>
-      <c r="G78" s="56"/>
-      <c r="H78" s="56"/>
-      <c r="I78" s="56"/>
+      <c r="B78" s="58"/>
+      <c r="C78" s="58"/>
+      <c r="D78" s="58"/>
+      <c r="E78" s="58"/>
+      <c r="F78" s="58"/>
+      <c r="G78" s="58"/>
+      <c r="H78" s="58"/>
+      <c r="I78" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="79">
-      <c r="B79" s="56"/>
-      <c r="C79" s="56"/>
-      <c r="D79" s="56"/>
-      <c r="E79" s="56"/>
-      <c r="F79" s="56"/>
-      <c r="G79" s="56"/>
-      <c r="H79" s="56"/>
-      <c r="I79" s="56"/>
+      <c r="B79" s="58"/>
+      <c r="C79" s="58"/>
+      <c r="D79" s="58"/>
+      <c r="E79" s="58"/>
+      <c r="F79" s="58"/>
+      <c r="G79" s="58"/>
+      <c r="H79" s="58"/>
+      <c r="I79" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="80">
-      <c r="B80" s="56"/>
-      <c r="C80" s="56"/>
-      <c r="D80" s="56"/>
-      <c r="E80" s="56"/>
-      <c r="F80" s="56"/>
-      <c r="G80" s="56"/>
-      <c r="H80" s="56"/>
-      <c r="I80" s="56"/>
+      <c r="B80" s="58"/>
+      <c r="C80" s="58"/>
+      <c r="D80" s="58"/>
+      <c r="E80" s="58"/>
+      <c r="F80" s="58"/>
+      <c r="G80" s="58"/>
+      <c r="H80" s="58"/>
+      <c r="I80" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="81">
-      <c r="B81" s="56"/>
-      <c r="C81" s="56"/>
-      <c r="D81" s="56"/>
-      <c r="E81" s="56"/>
-      <c r="F81" s="56"/>
-      <c r="G81" s="56"/>
-      <c r="H81" s="56"/>
-      <c r="I81" s="56"/>
+      <c r="B81" s="58"/>
+      <c r="C81" s="58"/>
+      <c r="D81" s="58"/>
+      <c r="E81" s="58"/>
+      <c r="F81" s="58"/>
+      <c r="G81" s="58"/>
+      <c r="H81" s="58"/>
+      <c r="I81" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="82">
-      <c r="B82" s="56"/>
-      <c r="C82" s="56"/>
-      <c r="D82" s="56"/>
-      <c r="E82" s="56"/>
-      <c r="F82" s="56"/>
-      <c r="G82" s="56"/>
-      <c r="H82" s="56"/>
-      <c r="I82" s="56"/>
+      <c r="B82" s="58"/>
+      <c r="C82" s="58"/>
+      <c r="D82" s="58"/>
+      <c r="E82" s="58"/>
+      <c r="F82" s="58"/>
+      <c r="G82" s="58"/>
+      <c r="H82" s="58"/>
+      <c r="I82" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="83">
-      <c r="B83" s="56"/>
-      <c r="C83" s="56"/>
-      <c r="D83" s="56"/>
-      <c r="E83" s="56"/>
-      <c r="F83" s="56"/>
-      <c r="G83" s="56"/>
-      <c r="H83" s="56"/>
-      <c r="I83" s="56"/>
+      <c r="B83" s="58"/>
+      <c r="C83" s="58"/>
+      <c r="D83" s="58"/>
+      <c r="E83" s="58"/>
+      <c r="F83" s="58"/>
+      <c r="G83" s="58"/>
+      <c r="H83" s="58"/>
+      <c r="I83" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="84">
-      <c r="B84" s="56"/>
-      <c r="C84" s="56"/>
-      <c r="D84" s="56"/>
-      <c r="E84" s="56"/>
-      <c r="F84" s="56"/>
-      <c r="G84" s="56"/>
-      <c r="H84" s="56"/>
-      <c r="I84" s="56"/>
+      <c r="B84" s="58"/>
+      <c r="C84" s="58"/>
+      <c r="D84" s="58"/>
+      <c r="E84" s="58"/>
+      <c r="F84" s="58"/>
+      <c r="G84" s="58"/>
+      <c r="H84" s="58"/>
+      <c r="I84" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="85">
-      <c r="B85" s="56"/>
-      <c r="C85" s="56"/>
-      <c r="D85" s="56"/>
-      <c r="E85" s="56"/>
-      <c r="F85" s="56"/>
-      <c r="G85" s="56"/>
-      <c r="H85" s="56"/>
-      <c r="I85" s="56"/>
+      <c r="B85" s="58"/>
+      <c r="C85" s="58"/>
+      <c r="D85" s="58"/>
+      <c r="E85" s="58"/>
+      <c r="F85" s="58"/>
+      <c r="G85" s="58"/>
+      <c r="H85" s="58"/>
+      <c r="I85" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="86">
-      <c r="B86" s="56"/>
-      <c r="C86" s="56"/>
-      <c r="D86" s="56"/>
-      <c r="E86" s="56"/>
-      <c r="F86" s="56"/>
-      <c r="G86" s="56"/>
-      <c r="H86" s="56"/>
-      <c r="I86" s="56"/>
+      <c r="B86" s="58"/>
+      <c r="C86" s="58"/>
+      <c r="D86" s="58"/>
+      <c r="E86" s="58"/>
+      <c r="F86" s="58"/>
+      <c r="G86" s="58"/>
+      <c r="H86" s="58"/>
+      <c r="I86" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87">
-      <c r="B87" s="56"/>
-      <c r="C87" s="56"/>
-      <c r="D87" s="56"/>
-      <c r="E87" s="56"/>
-      <c r="F87" s="56"/>
-      <c r="G87" s="56"/>
-      <c r="H87" s="56"/>
-      <c r="I87" s="56"/>
+      <c r="B87" s="58"/>
+      <c r="C87" s="58"/>
+      <c r="D87" s="58"/>
+      <c r="E87" s="58"/>
+      <c r="F87" s="58"/>
+      <c r="G87" s="58"/>
+      <c r="H87" s="58"/>
+      <c r="I87" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="88">
-      <c r="B88" s="56"/>
-      <c r="C88" s="56"/>
-      <c r="D88" s="56"/>
-      <c r="E88" s="56"/>
-      <c r="F88" s="56"/>
-      <c r="G88" s="56"/>
-      <c r="H88" s="56"/>
-      <c r="I88" s="56"/>
+      <c r="B88" s="58"/>
+      <c r="C88" s="58"/>
+      <c r="D88" s="58"/>
+      <c r="E88" s="58"/>
+      <c r="F88" s="58"/>
+      <c r="G88" s="58"/>
+      <c r="H88" s="58"/>
+      <c r="I88" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="89">
-      <c r="B89" s="56"/>
-      <c r="C89" s="56"/>
-      <c r="D89" s="56"/>
-      <c r="E89" s="56"/>
-      <c r="F89" s="56"/>
-      <c r="G89" s="56"/>
-      <c r="H89" s="56"/>
-      <c r="I89" s="56"/>
+      <c r="B89" s="58"/>
+      <c r="C89" s="58"/>
+      <c r="D89" s="58"/>
+      <c r="E89" s="58"/>
+      <c r="F89" s="58"/>
+      <c r="G89" s="58"/>
+      <c r="H89" s="58"/>
+      <c r="I89" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="90">
-      <c r="B90" s="56"/>
-      <c r="C90" s="56"/>
-      <c r="D90" s="56"/>
-      <c r="E90" s="56"/>
-      <c r="F90" s="56"/>
-      <c r="G90" s="56"/>
-      <c r="H90" s="56"/>
-      <c r="I90" s="56"/>
+      <c r="B90" s="58"/>
+      <c r="C90" s="58"/>
+      <c r="D90" s="58"/>
+      <c r="E90" s="58"/>
+      <c r="F90" s="58"/>
+      <c r="G90" s="58"/>
+      <c r="H90" s="58"/>
+      <c r="I90" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="91">
-      <c r="B91" s="56"/>
-      <c r="C91" s="56"/>
-      <c r="D91" s="56"/>
-      <c r="E91" s="56"/>
-      <c r="F91" s="56"/>
-      <c r="G91" s="56"/>
-      <c r="H91" s="56"/>
-      <c r="I91" s="56"/>
+      <c r="B91" s="58"/>
+      <c r="C91" s="58"/>
+      <c r="D91" s="58"/>
+      <c r="E91" s="58"/>
+      <c r="F91" s="58"/>
+      <c r="G91" s="58"/>
+      <c r="H91" s="58"/>
+      <c r="I91" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
-      <c r="B92" s="56"/>
-      <c r="C92" s="56"/>
-      <c r="D92" s="56"/>
-      <c r="E92" s="56"/>
-      <c r="F92" s="56"/>
-      <c r="G92" s="56"/>
-      <c r="H92" s="56"/>
-      <c r="I92" s="56"/>
+      <c r="B92" s="58"/>
+      <c r="C92" s="58"/>
+      <c r="D92" s="58"/>
+      <c r="E92" s="58"/>
+      <c r="F92" s="58"/>
+      <c r="G92" s="58"/>
+      <c r="H92" s="58"/>
+      <c r="I92" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93">
-      <c r="B93" s="56"/>
-      <c r="C93" s="56"/>
-      <c r="D93" s="56"/>
-      <c r="E93" s="56"/>
-      <c r="F93" s="56"/>
-      <c r="G93" s="56"/>
-      <c r="H93" s="56"/>
-      <c r="I93" s="56"/>
+      <c r="B93" s="58"/>
+      <c r="C93" s="58"/>
+      <c r="D93" s="58"/>
+      <c r="E93" s="58"/>
+      <c r="F93" s="58"/>
+      <c r="G93" s="58"/>
+      <c r="H93" s="58"/>
+      <c r="I93" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="94">
-      <c r="B94" s="56"/>
-      <c r="C94" s="56"/>
-      <c r="D94" s="56"/>
-      <c r="E94" s="56"/>
-      <c r="F94" s="56"/>
-      <c r="G94" s="56"/>
-      <c r="H94" s="56"/>
-      <c r="I94" s="56"/>
+      <c r="B94" s="58"/>
+      <c r="C94" s="58"/>
+      <c r="D94" s="58"/>
+      <c r="E94" s="58"/>
+      <c r="F94" s="58"/>
+      <c r="G94" s="58"/>
+      <c r="H94" s="58"/>
+      <c r="I94" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="95">
-      <c r="B95" s="56"/>
-      <c r="C95" s="56"/>
-      <c r="D95" s="56"/>
-      <c r="E95" s="56"/>
-      <c r="F95" s="56"/>
-      <c r="G95" s="56"/>
-      <c r="H95" s="56"/>
-      <c r="I95" s="56"/>
+      <c r="B95" s="58"/>
+      <c r="C95" s="58"/>
+      <c r="D95" s="58"/>
+      <c r="E95" s="58"/>
+      <c r="F95" s="58"/>
+      <c r="G95" s="58"/>
+      <c r="H95" s="58"/>
+      <c r="I95" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="96">
-      <c r="B96" s="56"/>
-      <c r="C96" s="56"/>
-      <c r="D96" s="56"/>
-      <c r="E96" s="56"/>
-      <c r="F96" s="56"/>
-      <c r="G96" s="56"/>
-      <c r="H96" s="56"/>
-      <c r="I96" s="56"/>
+      <c r="B96" s="58"/>
+      <c r="C96" s="58"/>
+      <c r="D96" s="58"/>
+      <c r="E96" s="58"/>
+      <c r="F96" s="58"/>
+      <c r="G96" s="58"/>
+      <c r="H96" s="58"/>
+      <c r="I96" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="97">
-      <c r="B97" s="56"/>
-      <c r="C97" s="56"/>
-      <c r="D97" s="56"/>
-      <c r="E97" s="56"/>
-      <c r="F97" s="56"/>
-      <c r="G97" s="56"/>
-      <c r="H97" s="56"/>
-      <c r="I97" s="56"/>
+      <c r="B97" s="58"/>
+      <c r="C97" s="58"/>
+      <c r="D97" s="58"/>
+      <c r="E97" s="58"/>
+      <c r="F97" s="58"/>
+      <c r="G97" s="58"/>
+      <c r="H97" s="58"/>
+      <c r="I97" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="98">
-      <c r="B98" s="56"/>
-      <c r="C98" s="56"/>
-      <c r="D98" s="56"/>
-      <c r="E98" s="56"/>
-      <c r="F98" s="56"/>
-      <c r="G98" s="56"/>
-      <c r="H98" s="56"/>
-      <c r="I98" s="56"/>
+      <c r="B98" s="58"/>
+      <c r="C98" s="58"/>
+      <c r="D98" s="58"/>
+      <c r="E98" s="58"/>
+      <c r="F98" s="58"/>
+      <c r="G98" s="58"/>
+      <c r="H98" s="58"/>
+      <c r="I98" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="99">
-      <c r="B99" s="56"/>
-      <c r="C99" s="56"/>
-      <c r="D99" s="56"/>
-      <c r="E99" s="56"/>
-      <c r="F99" s="56"/>
-      <c r="G99" s="56"/>
-      <c r="H99" s="56"/>
-      <c r="I99" s="56"/>
+      <c r="B99" s="58"/>
+      <c r="C99" s="58"/>
+      <c r="D99" s="58"/>
+      <c r="E99" s="58"/>
+      <c r="F99" s="58"/>
+      <c r="G99" s="58"/>
+      <c r="H99" s="58"/>
+      <c r="I99" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">
-      <c r="B100" s="56"/>
-      <c r="C100" s="56"/>
-      <c r="D100" s="56"/>
-      <c r="E100" s="56"/>
-      <c r="F100" s="56"/>
-      <c r="G100" s="56"/>
-      <c r="H100" s="56"/>
-      <c r="I100" s="56"/>
+      <c r="B100" s="58"/>
+      <c r="C100" s="58"/>
+      <c r="D100" s="58"/>
+      <c r="E100" s="58"/>
+      <c r="F100" s="58"/>
+      <c r="G100" s="58"/>
+      <c r="H100" s="58"/>
+      <c r="I100" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="101">
-      <c r="B101" s="56"/>
-      <c r="C101" s="56"/>
-      <c r="D101" s="56"/>
-      <c r="E101" s="56"/>
-      <c r="F101" s="56"/>
-      <c r="G101" s="56"/>
-      <c r="H101" s="56"/>
-      <c r="I101" s="56"/>
+      <c r="B101" s="58"/>
+      <c r="C101" s="58"/>
+      <c r="D101" s="58"/>
+      <c r="E101" s="58"/>
+      <c r="F101" s="58"/>
+      <c r="G101" s="58"/>
+      <c r="H101" s="58"/>
+      <c r="I101" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="102">
-      <c r="B102" s="56"/>
-      <c r="C102" s="56"/>
-      <c r="D102" s="56"/>
-      <c r="E102" s="56"/>
-      <c r="F102" s="56"/>
-      <c r="G102" s="56"/>
-      <c r="H102" s="56"/>
-      <c r="I102" s="56"/>
+      <c r="B102" s="58"/>
+      <c r="C102" s="58"/>
+      <c r="D102" s="58"/>
+      <c r="E102" s="58"/>
+      <c r="F102" s="58"/>
+      <c r="G102" s="58"/>
+      <c r="H102" s="58"/>
+      <c r="I102" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="103">
-      <c r="B103" s="56"/>
-      <c r="C103" s="56"/>
-      <c r="D103" s="56"/>
-      <c r="E103" s="56"/>
-      <c r="F103" s="56"/>
-      <c r="G103" s="56"/>
-      <c r="H103" s="56"/>
-      <c r="I103" s="56"/>
+      <c r="B103" s="58"/>
+      <c r="C103" s="58"/>
+      <c r="D103" s="58"/>
+      <c r="E103" s="58"/>
+      <c r="F103" s="58"/>
+      <c r="G103" s="58"/>
+      <c r="H103" s="58"/>
+      <c r="I103" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="104">
-      <c r="B104" s="56"/>
-      <c r="C104" s="56"/>
-      <c r="D104" s="56"/>
-      <c r="E104" s="56"/>
-      <c r="F104" s="56"/>
-      <c r="G104" s="56"/>
-      <c r="H104" s="56"/>
-      <c r="I104" s="56"/>
+      <c r="B104" s="58"/>
+      <c r="C104" s="58"/>
+      <c r="D104" s="58"/>
+      <c r="E104" s="58"/>
+      <c r="F104" s="58"/>
+      <c r="G104" s="58"/>
+      <c r="H104" s="58"/>
+      <c r="I104" s="58"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="105">
-      <c r="B105" s="56"/>
-      <c r="C105" s="56"/>
-      <c r="D105" s="56"/>
-      <c r="E105" s="56"/>
-      <c r="F105" s="56"/>
-      <c r="G105" s="56"/>
-      <c r="H105" s="56"/>
-      <c r="I105" s="56"/>
+      <c r="B105" s="58"/>
+      <c r="C105" s="58"/>
+      <c r="D105" s="58"/>
+      <c r="E105" s="58"/>
+      <c r="F105" s="58"/>
+      <c r="G105" s="58"/>
+      <c r="H105" s="58"/>
+      <c r="I105" s="58"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="106">
+      <c r="B106" s="58"/>
+      <c r="C106" s="58"/>
+      <c r="D106" s="58"/>
+      <c r="E106" s="58"/>
+      <c r="F106" s="58"/>
+      <c r="G106" s="58"/>
+      <c r="H106" s="58"/>
+      <c r="I106" s="58"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="107">
+      <c r="B107" s="58"/>
+      <c r="C107" s="58"/>
+      <c r="D107" s="58"/>
+      <c r="E107" s="58"/>
+      <c r="F107" s="58"/>
+      <c r="G107" s="58"/>
+      <c r="H107" s="58"/>
+      <c r="I107" s="58"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="108">
+      <c r="B108" s="58"/>
+      <c r="C108" s="58"/>
+      <c r="D108" s="58"/>
+      <c r="E108" s="58"/>
+      <c r="F108" s="58"/>
+      <c r="G108" s="58"/>
+      <c r="H108" s="58"/>
+      <c r="I108" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B45:D45"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2018,223 +2065,223 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.9647058823529"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.8313725490196"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7098039215686"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.1921568627451"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.7254901960784"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.4352941176471"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.0235294117647"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.8509803921569"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="41.243137254902"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.9647058823529"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.7529411764706"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.9647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0196078431373"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.0666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8627450980392"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.4078431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.843137254902"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.6352941176471"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.2039215686274"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.9882352941176"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="41.4509803921569"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.0196078431373"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.8313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="12.0196078431373"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="B2" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
-      <c r="A5" s="65" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="65" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="65" t="s">
+      <c r="A5" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="65" t="s">
+      <c r="C5" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" s="65" t="s">
+      <c r="D5" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="H5" s="65" t="s">
+      <c r="E5" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="65"/>
+      <c r="I5" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
-      <c r="A6" s="65" t="s">
-        <v>79</v>
-      </c>
-      <c r="B6" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="65" t="s">
+      <c r="A6" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="B6" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="C6" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="F6" s="65" t="s">
+      <c r="D6" s="67" t="s">
         <v>84</v>
       </c>
-      <c r="G6" s="65" t="s">
+      <c r="E6" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="H6" s="65" t="s">
+      <c r="F6" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="65" t="s">
+      <c r="G6" s="67" t="s">
         <v>87</v>
       </c>
+      <c r="H6" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" s="67" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="B7" s="66" t="s">
-        <v>88</v>
-      </c>
-      <c r="C7" s="67" t="s">
+      <c r="B7" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="66" t="s">
-        <v>89</v>
-      </c>
-      <c r="E7" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="F7" s="67" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="67" t="s">
+      <c r="D7" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="H7" s="67" t="s">
+      <c r="E7" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="I7" s="69" t="s">
+      <c r="F7" s="69" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="69" t="s">
         <v>93</v>
       </c>
+      <c r="H7" s="69" t="s">
+        <v>94</v>
+      </c>
+      <c r="I7" s="71" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
-      <c r="B8" s="66" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" s="67" t="s">
-        <v>95</v>
-      </c>
-      <c r="D8" s="66" t="s">
+      <c r="B8" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="E8" s="66" t="s">
+      <c r="C8" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="F8" s="66" t="s">
+      <c r="D8" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="H8" s="67" t="s">
+      <c r="E8" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="I8" s="69" t="s">
+      <c r="F8" s="68" t="s">
         <v>100</v>
       </c>
+      <c r="H8" s="69" t="s">
+        <v>101</v>
+      </c>
+      <c r="I8" s="71" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
-      <c r="B9" s="66" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="67" t="s">
-        <v>102</v>
-      </c>
-      <c r="D9" s="66" t="s">
+      <c r="B9" s="68" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="68" t="s">
+      <c r="C9" s="69" t="s">
         <v>104</v>
       </c>
-      <c r="F9" s="66" t="s">
+      <c r="D9" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="I9" s="69" t="s">
+      <c r="E9" s="70" t="s">
         <v>106</v>
       </c>
+      <c r="F9" s="68" t="s">
+        <v>107</v>
+      </c>
+      <c r="I9" s="71" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="67" t="s">
-        <v>107</v>
-      </c>
-      <c r="I10" s="69" t="s">
-        <v>108</v>
+      <c r="C10" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="I10" s="71" t="s">
+        <v>110</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
-      <c r="B11" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="C11" s="67" t="s">
-        <v>110</v>
-      </c>
-      <c r="I11" s="70" t="s">
+      <c r="B11" s="69" t="s">
         <v>111</v>
+      </c>
+      <c r="C11" s="69" t="s">
+        <v>112</v>
+      </c>
+      <c r="I11" s="72" t="s">
+        <v>113</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="B12" s="67" t="s">
-        <v>112</v>
-      </c>
-      <c r="C12" s="67" t="s">
-        <v>113</v>
-      </c>
-      <c r="I12" s="70" t="s">
+      <c r="B12" s="69" t="s">
         <v>114</v>
+      </c>
+      <c r="C12" s="69" t="s">
+        <v>115</v>
+      </c>
+      <c r="I12" s="72" t="s">
+        <v>116</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
-      <c r="B13" s="67" t="s">
-        <v>115</v>
-      </c>
-      <c r="I13" s="70" t="s">
-        <v>116</v>
+      <c r="B13" s="69" t="s">
+        <v>117</v>
+      </c>
+      <c r="I13" s="72" t="s">
+        <v>118</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="B14" s="67" t="s">
-        <v>117</v>
-      </c>
-      <c r="I14" s="70" t="s">
-        <v>118</v>
+      <c r="B14" s="69" t="s">
+        <v>119</v>
+      </c>
+      <c r="I14" s="72" t="s">
+        <v>120</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="69" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
-      <c r="B19" s="66" t="s">
-        <v>72</v>
+      <c r="B19" s="68" t="s">
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
-      <c r="B20" s="68" t="s">
-        <v>119</v>
+      <c r="B20" s="70" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
integrando calendario de respaldos y actualizacion de archivo plan de configuracion
</commit_message>
<xml_diff>
--- a/qualtcom/Organizacional/Configuracion/PlanConfiguracion.xlsx
+++ b/qualtcom/Organizacional/Configuracion/PlanConfiguracion.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="128">
   <si>
     <t>Plan de Administración de Configuración</t>
   </si>
@@ -165,6 +165,12 @@
     <t>Minuta_compromiso</t>
   </si>
   <si>
+    <t>Plan de actividad preventiva</t>
+  </si>
+  <si>
+    <t>Calendario_preventivo</t>
+  </si>
+  <si>
     <t>Catalogo de servicios</t>
   </si>
   <si>
@@ -183,7 +189,19 @@
     <t>Pólizas</t>
   </si>
   <si>
+    <t>Pólizas empresariales</t>
+  </si>
+  <si>
+    <t>VIA-Poliza</t>
+  </si>
+  <si>
     <t>Encuestas de satisfacción</t>
+  </si>
+  <si>
+    <t>Encuesta de Satisfacción</t>
+  </si>
+  <si>
+    <t>EncuestaSatisfaccion</t>
   </si>
   <si>
     <t>Linea Base</t>
@@ -765,7 +783,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
@@ -855,6 +873,9 @@
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="5" fontId="12" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="4" fontId="11" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
+    </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="10" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="true"/>
     </xf>
@@ -999,57 +1020,57 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I108"/>
+  <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A5" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C10" activeCellId="0" pane="topLeft" sqref="C10"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="false" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A23" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C34" activeCellId="0" pane="topLeft" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="2.82352941176471"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.0352941176471"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.8196078431373"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="68.4313725490196"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.6039215686274"/>
-    <col collapsed="false" hidden="false" max="251" min="6" style="1" width="12.0196078431373"/>
-    <col collapsed="false" hidden="false" max="252" min="252" style="1" width="2.82352941176471"/>
-    <col collapsed="false" hidden="false" max="253" min="253" style="1" width="48.4509803921569"/>
-    <col collapsed="false" hidden="false" max="254" min="254" style="1" width="60.7137254901961"/>
-    <col collapsed="false" hidden="false" max="255" min="255" style="1" width="31.9882352941176"/>
-    <col collapsed="false" hidden="false" max="256" min="256" style="1" width="11.5411764705882"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="2.85882352941176"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="51.8078431372549"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.5529411764706"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="69.4588235294118"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="23.956862745098"/>
+    <col collapsed="false" hidden="false" max="251" min="6" style="1" width="12.2"/>
+    <col collapsed="false" hidden="false" max="252" min="252" style="1" width="2.85882352941176"/>
+    <col collapsed="false" hidden="false" max="253" min="253" style="1" width="49.1843137254902"/>
+    <col collapsed="false" hidden="false" max="254" min="254" style="1" width="61.6196078431373"/>
+    <col collapsed="false" hidden="false" max="255" min="255" style="1" width="32.4705882352941"/>
+    <col collapsed="false" hidden="false" max="256" min="256" style="1" width="11.7137254901961"/>
     <col collapsed="false" hidden="false" max="257" min="257" style="1" width="1.12941176470588"/>
-    <col collapsed="false" hidden="false" max="258" min="258" style="1" width="28.4823529411765"/>
-    <col collapsed="false" hidden="false" max="259" min="259" style="1" width="23.6039215686274"/>
-    <col collapsed="false" hidden="false" max="260" min="260" style="1" width="2.43137254901961"/>
-    <col collapsed="false" hidden="false" max="261" min="261" style="1" width="23.6039215686274"/>
-    <col collapsed="false" hidden="false" max="507" min="262" style="1" width="12.0196078431373"/>
-    <col collapsed="false" hidden="false" max="508" min="508" style="1" width="2.82352941176471"/>
-    <col collapsed="false" hidden="false" max="509" min="509" style="1" width="48.4509803921569"/>
-    <col collapsed="false" hidden="false" max="510" min="510" style="1" width="60.7137254901961"/>
-    <col collapsed="false" hidden="false" max="511" min="511" style="1" width="31.9882352941176"/>
-    <col collapsed="false" hidden="false" max="512" min="512" style="1" width="11.5411764705882"/>
+    <col collapsed="false" hidden="false" max="258" min="258" style="1" width="28.9058823529412"/>
+    <col collapsed="false" hidden="false" max="259" min="259" style="1" width="23.956862745098"/>
+    <col collapsed="false" hidden="false" max="260" min="260" style="1" width="2.47058823529412"/>
+    <col collapsed="false" hidden="false" max="261" min="261" style="1" width="23.956862745098"/>
+    <col collapsed="false" hidden="false" max="507" min="262" style="1" width="12.2"/>
+    <col collapsed="false" hidden="false" max="508" min="508" style="1" width="2.85882352941176"/>
+    <col collapsed="false" hidden="false" max="509" min="509" style="1" width="49.1843137254902"/>
+    <col collapsed="false" hidden="false" max="510" min="510" style="1" width="61.6196078431373"/>
+    <col collapsed="false" hidden="false" max="511" min="511" style="1" width="32.4705882352941"/>
+    <col collapsed="false" hidden="false" max="512" min="512" style="1" width="11.7137254901961"/>
     <col collapsed="false" hidden="false" max="513" min="513" style="1" width="1.12941176470588"/>
-    <col collapsed="false" hidden="false" max="514" min="514" style="1" width="28.4823529411765"/>
-    <col collapsed="false" hidden="false" max="515" min="515" style="1" width="23.6039215686274"/>
-    <col collapsed="false" hidden="false" max="516" min="516" style="1" width="2.43137254901961"/>
-    <col collapsed="false" hidden="false" max="517" min="517" style="1" width="23.6039215686274"/>
-    <col collapsed="false" hidden="false" max="763" min="518" style="1" width="12.0196078431373"/>
-    <col collapsed="false" hidden="false" max="764" min="764" style="1" width="2.82352941176471"/>
-    <col collapsed="false" hidden="false" max="765" min="765" style="1" width="48.4509803921569"/>
-    <col collapsed="false" hidden="false" max="766" min="766" style="1" width="60.7137254901961"/>
-    <col collapsed="false" hidden="false" max="767" min="767" style="1" width="31.9882352941176"/>
-    <col collapsed="false" hidden="false" max="768" min="768" style="1" width="11.5411764705882"/>
+    <col collapsed="false" hidden="false" max="514" min="514" style="1" width="28.9058823529412"/>
+    <col collapsed="false" hidden="false" max="515" min="515" style="1" width="23.956862745098"/>
+    <col collapsed="false" hidden="false" max="516" min="516" style="1" width="2.47058823529412"/>
+    <col collapsed="false" hidden="false" max="517" min="517" style="1" width="23.956862745098"/>
+    <col collapsed="false" hidden="false" max="763" min="518" style="1" width="12.2"/>
+    <col collapsed="false" hidden="false" max="764" min="764" style="1" width="2.85882352941176"/>
+    <col collapsed="false" hidden="false" max="765" min="765" style="1" width="49.1843137254902"/>
+    <col collapsed="false" hidden="false" max="766" min="766" style="1" width="61.6196078431373"/>
+    <col collapsed="false" hidden="false" max="767" min="767" style="1" width="32.4705882352941"/>
+    <col collapsed="false" hidden="false" max="768" min="768" style="1" width="11.7137254901961"/>
     <col collapsed="false" hidden="false" max="769" min="769" style="1" width="1.12941176470588"/>
-    <col collapsed="false" hidden="false" max="770" min="770" style="1" width="28.4823529411765"/>
-    <col collapsed="false" hidden="false" max="771" min="771" style="1" width="23.6039215686274"/>
-    <col collapsed="false" hidden="false" max="772" min="772" style="1" width="2.43137254901961"/>
-    <col collapsed="false" hidden="false" max="773" min="773" style="1" width="23.6039215686274"/>
-    <col collapsed="false" hidden="false" max="1019" min="774" style="1" width="12.0196078431373"/>
-    <col collapsed="false" hidden="false" max="1020" min="1020" style="1" width="2.82352941176471"/>
-    <col collapsed="false" hidden="false" max="1021" min="1021" style="1" width="48.4509803921569"/>
-    <col collapsed="false" hidden="false" max="1022" min="1022" style="1" width="60.7137254901961"/>
-    <col collapsed="false" hidden="false" max="1023" min="1023" style="1" width="31.9882352941176"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="11.5411764705882"/>
+    <col collapsed="false" hidden="false" max="770" min="770" style="1" width="28.9058823529412"/>
+    <col collapsed="false" hidden="false" max="771" min="771" style="1" width="23.956862745098"/>
+    <col collapsed="false" hidden="false" max="772" min="772" style="1" width="2.47058823529412"/>
+    <col collapsed="false" hidden="false" max="773" min="773" style="1" width="23.956862745098"/>
+    <col collapsed="false" hidden="false" max="1019" min="774" style="1" width="12.2"/>
+    <col collapsed="false" hidden="false" max="1020" min="1020" style="1" width="2.85882352941176"/>
+    <col collapsed="false" hidden="false" max="1021" min="1021" style="1" width="49.1843137254902"/>
+    <col collapsed="false" hidden="false" max="1022" min="1022" style="1" width="61.6196078431373"/>
+    <col collapsed="false" hidden="false" max="1023" min="1023" style="1" width="32.4705882352941"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="1" width="11.7137254901961"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="1">
@@ -1374,674 +1395,683 @@
       <c r="B35" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="43" t="s">
         <v>48</v>
       </c>
       <c r="D35" s="34"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="36">
-      <c r="B36" s="35" t="s">
+      <c r="B36" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="34"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="37">
+      <c r="B37" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="36"/>
-      <c r="D36" s="37"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="37">
-      <c r="B37" s="26" t="s">
+      <c r="C37" s="36"/>
+      <c r="D37" s="37"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
+      <c r="B38" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C37" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="D37" s="38"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="38">
-      <c r="B38" s="35" t="s">
+      <c r="C38" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" s="38"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="39">
+      <c r="B39" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="36"/>
-      <c r="D38" s="37"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="39">
-      <c r="A39" s="6"/>
-      <c r="B39" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D39" s="15" t="s">
+      <c r="C39" s="36"/>
+      <c r="D39" s="37"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="40">
+      <c r="A40" s="6"/>
+      <c r="B40" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="40">
-      <c r="B40" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="C40" s="36"/>
-      <c r="D40" s="37"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="41">
-      <c r="A41" s="6"/>
-      <c r="B41" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" s="15" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="41">
+      <c r="B41" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="36"/>
+      <c r="D41" s="37"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="42">
+      <c r="A42" s="6"/>
+      <c r="B42" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="42">
-      <c r="B42" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42" s="36"/>
-      <c r="D42" s="37"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="43">
-      <c r="A43" s="6"/>
-      <c r="B43" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D43" s="15" t="s">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="43">
+      <c r="B43" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C43" s="36"/>
+      <c r="D43" s="37"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="44">
+      <c r="A44" s="6"/>
+      <c r="B44" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="44" s="40">
-      <c r="B44" s="43"/>
-      <c r="C44" s="43"/>
-      <c r="D44" s="43"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="45">
-      <c r="B45" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
+    <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.5" outlineLevel="0" r="45" s="40">
+      <c r="B45" s="44"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="46">
-      <c r="B46" s="44" t="s">
-        <v>55</v>
-      </c>
-      <c r="C46" s="44" t="s">
-        <v>56</v>
-      </c>
-      <c r="D46" s="44" t="s">
-        <v>57</v>
-      </c>
+      <c r="B46" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="47">
       <c r="B47" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="C47" s="46"/>
-      <c r="D47" s="47"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="48">
-      <c r="B48" s="48" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="D47" s="45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="48">
+      <c r="B48" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="47"/>
+      <c r="D48" s="48"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.65" outlineLevel="0" r="49">
+      <c r="B49" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="48" t="s">
-        <v>58</v>
-      </c>
-      <c r="D48" s="49" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="49">
-      <c r="B49" s="50"/>
-      <c r="C49" s="50"/>
-      <c r="D49" s="51"/>
+      <c r="C49" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="D49" s="50" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="50">
-      <c r="A50" s="52"/>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="51"/>
+      <c r="C50" s="51"/>
+      <c r="D50" s="52"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15" outlineLevel="0" r="51">
+      <c r="A51" s="53"/>
+      <c r="B51" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C50" s="9"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="51">
-      <c r="B51" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="C51" s="54"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="52">
-      <c r="B52" s="55" t="s">
-        <v>61</v>
-      </c>
-      <c r="C52" s="56"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="53">
-      <c r="B53" s="57"/>
-      <c r="C53" s="58"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="54">
-      <c r="A54" s="52"/>
-      <c r="B54" s="59" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" s="10"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="1" r="55">
+      <c r="C51" s="9"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="52">
+      <c r="B52" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="55"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="25.35" outlineLevel="0" r="53">
+      <c r="B53" s="56" t="s">
+        <v>67</v>
+      </c>
+      <c r="C53" s="57"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="54">
+      <c r="B54" s="58"/>
+      <c r="C54" s="59"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="55">
+      <c r="A55" s="53"/>
       <c r="B55" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="C55" s="61"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="1" r="56">
-      <c r="B56" s="62"/>
+        <v>68</v>
+      </c>
+      <c r="C55" s="10"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="57.45" outlineLevel="1" r="56">
+      <c r="B56" s="61" t="s">
+        <v>69</v>
+      </c>
       <c r="C56" s="62"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="1" r="57">
-      <c r="B57" s="62"/>
-      <c r="C57" s="62"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="58">
-      <c r="A58" s="58"/>
+      <c r="B57" s="63"/>
+      <c r="C57" s="63"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="1" r="58">
       <c r="B58" s="63"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="58"/>
+      <c r="C58" s="63"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="59">
+      <c r="A59" s="59"/>
       <c r="B59" s="64"/>
-      <c r="C59" s="58"/>
-      <c r="D59" s="58"/>
+      <c r="C59" s="59"/>
+      <c r="D59" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="60">
-      <c r="B60" s="58"/>
-      <c r="C60" s="58"/>
-      <c r="D60" s="58"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="61">
-      <c r="A61" s="52"/>
-      <c r="B61" s="59" t="s">
-        <v>64</v>
-      </c>
-      <c r="C61" s="59" t="s">
-        <v>65</v>
-      </c>
-      <c r="D61" s="59" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="62">
-      <c r="B62" s="65" t="s">
-        <v>67</v>
-      </c>
-      <c r="C62" s="65" t="s">
-        <v>68</v>
-      </c>
-      <c r="D62" s="65" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="63">
-      <c r="B63" s="65" t="s">
+      <c r="B60" s="65"/>
+      <c r="C60" s="59"/>
+      <c r="D60" s="59"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="61">
+      <c r="B61" s="59"/>
+      <c r="C61" s="59"/>
+      <c r="D61" s="59"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.9" outlineLevel="0" r="62">
+      <c r="A62" s="53"/>
+      <c r="B62" s="60" t="s">
         <v>70</v>
       </c>
-      <c r="C63" s="65" t="s">
+      <c r="C62" s="60" t="s">
         <v>71</v>
       </c>
+      <c r="D62" s="60" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="63">
+      <c r="B63" s="66" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" s="66" t="s">
+        <v>74</v>
+      </c>
       <c r="D63" s="66" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="64">
-      <c r="B64" s="62"/>
-      <c r="C64" s="62"/>
-      <c r="D64" s="62"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="64">
+      <c r="B64" s="66" t="s">
+        <v>76</v>
+      </c>
+      <c r="C64" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="D64" s="67" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="65">
-      <c r="B65" s="58"/>
-      <c r="C65" s="58"/>
-      <c r="D65" s="58"/>
-      <c r="E65" s="58"/>
-      <c r="F65" s="58"/>
-      <c r="G65" s="58"/>
-      <c r="H65" s="58"/>
-      <c r="I65" s="58"/>
+      <c r="B65" s="63"/>
+      <c r="C65" s="63"/>
+      <c r="D65" s="63"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="66">
-      <c r="B66" s="58"/>
-      <c r="C66" s="58"/>
-      <c r="D66" s="58"/>
-      <c r="E66" s="58"/>
-      <c r="F66" s="58"/>
-      <c r="G66" s="58"/>
-      <c r="H66" s="58"/>
-      <c r="I66" s="58"/>
+      <c r="B66" s="59"/>
+      <c r="C66" s="59"/>
+      <c r="D66" s="59"/>
+      <c r="E66" s="59"/>
+      <c r="F66" s="59"/>
+      <c r="G66" s="59"/>
+      <c r="H66" s="59"/>
+      <c r="I66" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="67">
-      <c r="B67" s="58"/>
-      <c r="C67" s="58"/>
-      <c r="D67" s="58"/>
-      <c r="E67" s="58"/>
-      <c r="F67" s="58"/>
-      <c r="G67" s="58"/>
-      <c r="H67" s="58"/>
-      <c r="I67" s="58"/>
+      <c r="B67" s="59"/>
+      <c r="C67" s="59"/>
+      <c r="D67" s="59"/>
+      <c r="E67" s="59"/>
+      <c r="F67" s="59"/>
+      <c r="G67" s="59"/>
+      <c r="H67" s="59"/>
+      <c r="I67" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="68">
-      <c r="B68" s="58"/>
-      <c r="C68" s="58"/>
-      <c r="D68" s="58"/>
-      <c r="E68" s="58"/>
-      <c r="F68" s="58"/>
-      <c r="G68" s="58"/>
-      <c r="H68" s="58"/>
-      <c r="I68" s="58"/>
+      <c r="B68" s="59"/>
+      <c r="C68" s="59"/>
+      <c r="D68" s="59"/>
+      <c r="E68" s="59"/>
+      <c r="F68" s="59"/>
+      <c r="G68" s="59"/>
+      <c r="H68" s="59"/>
+      <c r="I68" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="69">
-      <c r="B69" s="58"/>
-      <c r="C69" s="58"/>
-      <c r="D69" s="58"/>
-      <c r="E69" s="58"/>
-      <c r="F69" s="58"/>
-      <c r="G69" s="58"/>
-      <c r="H69" s="58"/>
-      <c r="I69" s="58"/>
+      <c r="B69" s="59"/>
+      <c r="C69" s="59"/>
+      <c r="D69" s="59"/>
+      <c r="E69" s="59"/>
+      <c r="F69" s="59"/>
+      <c r="G69" s="59"/>
+      <c r="H69" s="59"/>
+      <c r="I69" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="70">
-      <c r="B70" s="58"/>
-      <c r="C70" s="58"/>
-      <c r="D70" s="58"/>
-      <c r="E70" s="58"/>
-      <c r="F70" s="58"/>
-      <c r="G70" s="58"/>
-      <c r="H70" s="58"/>
-      <c r="I70" s="58"/>
+      <c r="B70" s="59"/>
+      <c r="C70" s="59"/>
+      <c r="D70" s="59"/>
+      <c r="E70" s="59"/>
+      <c r="F70" s="59"/>
+      <c r="G70" s="59"/>
+      <c r="H70" s="59"/>
+      <c r="I70" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="71">
-      <c r="B71" s="58"/>
-      <c r="C71" s="58"/>
-      <c r="D71" s="58"/>
-      <c r="E71" s="58"/>
-      <c r="F71" s="58"/>
-      <c r="G71" s="58"/>
-      <c r="H71" s="58"/>
-      <c r="I71" s="58"/>
+      <c r="B71" s="59"/>
+      <c r="C71" s="59"/>
+      <c r="D71" s="59"/>
+      <c r="E71" s="59"/>
+      <c r="F71" s="59"/>
+      <c r="G71" s="59"/>
+      <c r="H71" s="59"/>
+      <c r="I71" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="72">
-      <c r="B72" s="58"/>
-      <c r="C72" s="58"/>
-      <c r="D72" s="58"/>
-      <c r="E72" s="58"/>
-      <c r="F72" s="58"/>
-      <c r="G72" s="58"/>
-      <c r="H72" s="58"/>
-      <c r="I72" s="58"/>
+      <c r="B72" s="59"/>
+      <c r="C72" s="59"/>
+      <c r="D72" s="59"/>
+      <c r="E72" s="59"/>
+      <c r="F72" s="59"/>
+      <c r="G72" s="59"/>
+      <c r="H72" s="59"/>
+      <c r="I72" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="73">
-      <c r="B73" s="58"/>
-      <c r="C73" s="58"/>
-      <c r="D73" s="58"/>
-      <c r="E73" s="58"/>
-      <c r="F73" s="58"/>
-      <c r="G73" s="58"/>
-      <c r="H73" s="58"/>
-      <c r="I73" s="58"/>
+      <c r="B73" s="59"/>
+      <c r="C73" s="59"/>
+      <c r="D73" s="59"/>
+      <c r="E73" s="59"/>
+      <c r="F73" s="59"/>
+      <c r="G73" s="59"/>
+      <c r="H73" s="59"/>
+      <c r="I73" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="74">
-      <c r="B74" s="58"/>
-      <c r="C74" s="58"/>
-      <c r="D74" s="58"/>
-      <c r="E74" s="58"/>
-      <c r="F74" s="58"/>
-      <c r="G74" s="58"/>
-      <c r="H74" s="58"/>
-      <c r="I74" s="58"/>
+      <c r="B74" s="59"/>
+      <c r="C74" s="59"/>
+      <c r="D74" s="59"/>
+      <c r="E74" s="59"/>
+      <c r="F74" s="59"/>
+      <c r="G74" s="59"/>
+      <c r="H74" s="59"/>
+      <c r="I74" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="75">
-      <c r="B75" s="58"/>
-      <c r="C75" s="58"/>
-      <c r="D75" s="58"/>
-      <c r="E75" s="58"/>
-      <c r="F75" s="58"/>
-      <c r="G75" s="58"/>
-      <c r="H75" s="58"/>
-      <c r="I75" s="58"/>
+      <c r="B75" s="59"/>
+      <c r="C75" s="59"/>
+      <c r="D75" s="59"/>
+      <c r="E75" s="59"/>
+      <c r="F75" s="59"/>
+      <c r="G75" s="59"/>
+      <c r="H75" s="59"/>
+      <c r="I75" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="76">
-      <c r="B76" s="58"/>
-      <c r="C76" s="58"/>
-      <c r="D76" s="58"/>
-      <c r="E76" s="58"/>
-      <c r="F76" s="58"/>
-      <c r="G76" s="58"/>
-      <c r="H76" s="58"/>
-      <c r="I76" s="58"/>
+      <c r="B76" s="59"/>
+      <c r="C76" s="59"/>
+      <c r="D76" s="59"/>
+      <c r="E76" s="59"/>
+      <c r="F76" s="59"/>
+      <c r="G76" s="59"/>
+      <c r="H76" s="59"/>
+      <c r="I76" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="77">
-      <c r="B77" s="58"/>
-      <c r="C77" s="58"/>
-      <c r="D77" s="58"/>
-      <c r="E77" s="58"/>
-      <c r="F77" s="58"/>
-      <c r="G77" s="58"/>
-      <c r="H77" s="58"/>
-      <c r="I77" s="58"/>
+      <c r="B77" s="59"/>
+      <c r="C77" s="59"/>
+      <c r="D77" s="59"/>
+      <c r="E77" s="59"/>
+      <c r="F77" s="59"/>
+      <c r="G77" s="59"/>
+      <c r="H77" s="59"/>
+      <c r="I77" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="78">
-      <c r="B78" s="58"/>
-      <c r="C78" s="58"/>
-      <c r="D78" s="58"/>
-      <c r="E78" s="58"/>
-      <c r="F78" s="58"/>
-      <c r="G78" s="58"/>
-      <c r="H78" s="58"/>
-      <c r="I78" s="58"/>
+      <c r="B78" s="59"/>
+      <c r="C78" s="59"/>
+      <c r="D78" s="59"/>
+      <c r="E78" s="59"/>
+      <c r="F78" s="59"/>
+      <c r="G78" s="59"/>
+      <c r="H78" s="59"/>
+      <c r="I78" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="79">
-      <c r="B79" s="58"/>
-      <c r="C79" s="58"/>
-      <c r="D79" s="58"/>
-      <c r="E79" s="58"/>
-      <c r="F79" s="58"/>
-      <c r="G79" s="58"/>
-      <c r="H79" s="58"/>
-      <c r="I79" s="58"/>
+      <c r="B79" s="59"/>
+      <c r="C79" s="59"/>
+      <c r="D79" s="59"/>
+      <c r="E79" s="59"/>
+      <c r="F79" s="59"/>
+      <c r="G79" s="59"/>
+      <c r="H79" s="59"/>
+      <c r="I79" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="80">
-      <c r="B80" s="58"/>
-      <c r="C80" s="58"/>
-      <c r="D80" s="58"/>
-      <c r="E80" s="58"/>
-      <c r="F80" s="58"/>
-      <c r="G80" s="58"/>
-      <c r="H80" s="58"/>
-      <c r="I80" s="58"/>
+      <c r="B80" s="59"/>
+      <c r="C80" s="59"/>
+      <c r="D80" s="59"/>
+      <c r="E80" s="59"/>
+      <c r="F80" s="59"/>
+      <c r="G80" s="59"/>
+      <c r="H80" s="59"/>
+      <c r="I80" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="81">
-      <c r="B81" s="58"/>
-      <c r="C81" s="58"/>
-      <c r="D81" s="58"/>
-      <c r="E81" s="58"/>
-      <c r="F81" s="58"/>
-      <c r="G81" s="58"/>
-      <c r="H81" s="58"/>
-      <c r="I81" s="58"/>
+      <c r="B81" s="59"/>
+      <c r="C81" s="59"/>
+      <c r="D81" s="59"/>
+      <c r="E81" s="59"/>
+      <c r="F81" s="59"/>
+      <c r="G81" s="59"/>
+      <c r="H81" s="59"/>
+      <c r="I81" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="82">
-      <c r="B82" s="58"/>
-      <c r="C82" s="58"/>
-      <c r="D82" s="58"/>
-      <c r="E82" s="58"/>
-      <c r="F82" s="58"/>
-      <c r="G82" s="58"/>
-      <c r="H82" s="58"/>
-      <c r="I82" s="58"/>
+      <c r="B82" s="59"/>
+      <c r="C82" s="59"/>
+      <c r="D82" s="59"/>
+      <c r="E82" s="59"/>
+      <c r="F82" s="59"/>
+      <c r="G82" s="59"/>
+      <c r="H82" s="59"/>
+      <c r="I82" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="83">
-      <c r="B83" s="58"/>
-      <c r="C83" s="58"/>
-      <c r="D83" s="58"/>
-      <c r="E83" s="58"/>
-      <c r="F83" s="58"/>
-      <c r="G83" s="58"/>
-      <c r="H83" s="58"/>
-      <c r="I83" s="58"/>
+      <c r="B83" s="59"/>
+      <c r="C83" s="59"/>
+      <c r="D83" s="59"/>
+      <c r="E83" s="59"/>
+      <c r="F83" s="59"/>
+      <c r="G83" s="59"/>
+      <c r="H83" s="59"/>
+      <c r="I83" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="84">
-      <c r="B84" s="58"/>
-      <c r="C84" s="58"/>
-      <c r="D84" s="58"/>
-      <c r="E84" s="58"/>
-      <c r="F84" s="58"/>
-      <c r="G84" s="58"/>
-      <c r="H84" s="58"/>
-      <c r="I84" s="58"/>
+      <c r="B84" s="59"/>
+      <c r="C84" s="59"/>
+      <c r="D84" s="59"/>
+      <c r="E84" s="59"/>
+      <c r="F84" s="59"/>
+      <c r="G84" s="59"/>
+      <c r="H84" s="59"/>
+      <c r="I84" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="85">
-      <c r="B85" s="58"/>
-      <c r="C85" s="58"/>
-      <c r="D85" s="58"/>
-      <c r="E85" s="58"/>
-      <c r="F85" s="58"/>
-      <c r="G85" s="58"/>
-      <c r="H85" s="58"/>
-      <c r="I85" s="58"/>
+      <c r="B85" s="59"/>
+      <c r="C85" s="59"/>
+      <c r="D85" s="59"/>
+      <c r="E85" s="59"/>
+      <c r="F85" s="59"/>
+      <c r="G85" s="59"/>
+      <c r="H85" s="59"/>
+      <c r="I85" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="86">
-      <c r="B86" s="58"/>
-      <c r="C86" s="58"/>
-      <c r="D86" s="58"/>
-      <c r="E86" s="58"/>
-      <c r="F86" s="58"/>
-      <c r="G86" s="58"/>
-      <c r="H86" s="58"/>
-      <c r="I86" s="58"/>
+      <c r="B86" s="59"/>
+      <c r="C86" s="59"/>
+      <c r="D86" s="59"/>
+      <c r="E86" s="59"/>
+      <c r="F86" s="59"/>
+      <c r="G86" s="59"/>
+      <c r="H86" s="59"/>
+      <c r="I86" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="87">
-      <c r="B87" s="58"/>
-      <c r="C87" s="58"/>
-      <c r="D87" s="58"/>
-      <c r="E87" s="58"/>
-      <c r="F87" s="58"/>
-      <c r="G87" s="58"/>
-      <c r="H87" s="58"/>
-      <c r="I87" s="58"/>
+      <c r="B87" s="59"/>
+      <c r="C87" s="59"/>
+      <c r="D87" s="59"/>
+      <c r="E87" s="59"/>
+      <c r="F87" s="59"/>
+      <c r="G87" s="59"/>
+      <c r="H87" s="59"/>
+      <c r="I87" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="88">
-      <c r="B88" s="58"/>
-      <c r="C88" s="58"/>
-      <c r="D88" s="58"/>
-      <c r="E88" s="58"/>
-      <c r="F88" s="58"/>
-      <c r="G88" s="58"/>
-      <c r="H88" s="58"/>
-      <c r="I88" s="58"/>
+      <c r="B88" s="59"/>
+      <c r="C88" s="59"/>
+      <c r="D88" s="59"/>
+      <c r="E88" s="59"/>
+      <c r="F88" s="59"/>
+      <c r="G88" s="59"/>
+      <c r="H88" s="59"/>
+      <c r="I88" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="89">
-      <c r="B89" s="58"/>
-      <c r="C89" s="58"/>
-      <c r="D89" s="58"/>
-      <c r="E89" s="58"/>
-      <c r="F89" s="58"/>
-      <c r="G89" s="58"/>
-      <c r="H89" s="58"/>
-      <c r="I89" s="58"/>
+      <c r="B89" s="59"/>
+      <c r="C89" s="59"/>
+      <c r="D89" s="59"/>
+      <c r="E89" s="59"/>
+      <c r="F89" s="59"/>
+      <c r="G89" s="59"/>
+      <c r="H89" s="59"/>
+      <c r="I89" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="90">
-      <c r="B90" s="58"/>
-      <c r="C90" s="58"/>
-      <c r="D90" s="58"/>
-      <c r="E90" s="58"/>
-      <c r="F90" s="58"/>
-      <c r="G90" s="58"/>
-      <c r="H90" s="58"/>
-      <c r="I90" s="58"/>
+      <c r="B90" s="59"/>
+      <c r="C90" s="59"/>
+      <c r="D90" s="59"/>
+      <c r="E90" s="59"/>
+      <c r="F90" s="59"/>
+      <c r="G90" s="59"/>
+      <c r="H90" s="59"/>
+      <c r="I90" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="91">
-      <c r="B91" s="58"/>
-      <c r="C91" s="58"/>
-      <c r="D91" s="58"/>
-      <c r="E91" s="58"/>
-      <c r="F91" s="58"/>
-      <c r="G91" s="58"/>
-      <c r="H91" s="58"/>
-      <c r="I91" s="58"/>
+      <c r="B91" s="59"/>
+      <c r="C91" s="59"/>
+      <c r="D91" s="59"/>
+      <c r="E91" s="59"/>
+      <c r="F91" s="59"/>
+      <c r="G91" s="59"/>
+      <c r="H91" s="59"/>
+      <c r="I91" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="92">
-      <c r="B92" s="58"/>
-      <c r="C92" s="58"/>
-      <c r="D92" s="58"/>
-      <c r="E92" s="58"/>
-      <c r="F92" s="58"/>
-      <c r="G92" s="58"/>
-      <c r="H92" s="58"/>
-      <c r="I92" s="58"/>
+      <c r="B92" s="59"/>
+      <c r="C92" s="59"/>
+      <c r="D92" s="59"/>
+      <c r="E92" s="59"/>
+      <c r="F92" s="59"/>
+      <c r="G92" s="59"/>
+      <c r="H92" s="59"/>
+      <c r="I92" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="93">
-      <c r="B93" s="58"/>
-      <c r="C93" s="58"/>
-      <c r="D93" s="58"/>
-      <c r="E93" s="58"/>
-      <c r="F93" s="58"/>
-      <c r="G93" s="58"/>
-      <c r="H93" s="58"/>
-      <c r="I93" s="58"/>
+      <c r="B93" s="59"/>
+      <c r="C93" s="59"/>
+      <c r="D93" s="59"/>
+      <c r="E93" s="59"/>
+      <c r="F93" s="59"/>
+      <c r="G93" s="59"/>
+      <c r="H93" s="59"/>
+      <c r="I93" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="94">
-      <c r="B94" s="58"/>
-      <c r="C94" s="58"/>
-      <c r="D94" s="58"/>
-      <c r="E94" s="58"/>
-      <c r="F94" s="58"/>
-      <c r="G94" s="58"/>
-      <c r="H94" s="58"/>
-      <c r="I94" s="58"/>
+      <c r="B94" s="59"/>
+      <c r="C94" s="59"/>
+      <c r="D94" s="59"/>
+      <c r="E94" s="59"/>
+      <c r="F94" s="59"/>
+      <c r="G94" s="59"/>
+      <c r="H94" s="59"/>
+      <c r="I94" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="95">
-      <c r="B95" s="58"/>
-      <c r="C95" s="58"/>
-      <c r="D95" s="58"/>
-      <c r="E95" s="58"/>
-      <c r="F95" s="58"/>
-      <c r="G95" s="58"/>
-      <c r="H95" s="58"/>
-      <c r="I95" s="58"/>
+      <c r="B95" s="59"/>
+      <c r="C95" s="59"/>
+      <c r="D95" s="59"/>
+      <c r="E95" s="59"/>
+      <c r="F95" s="59"/>
+      <c r="G95" s="59"/>
+      <c r="H95" s="59"/>
+      <c r="I95" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="96">
-      <c r="B96" s="58"/>
-      <c r="C96" s="58"/>
-      <c r="D96" s="58"/>
-      <c r="E96" s="58"/>
-      <c r="F96" s="58"/>
-      <c r="G96" s="58"/>
-      <c r="H96" s="58"/>
-      <c r="I96" s="58"/>
+      <c r="B96" s="59"/>
+      <c r="C96" s="59"/>
+      <c r="D96" s="59"/>
+      <c r="E96" s="59"/>
+      <c r="F96" s="59"/>
+      <c r="G96" s="59"/>
+      <c r="H96" s="59"/>
+      <c r="I96" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="97">
-      <c r="B97" s="58"/>
-      <c r="C97" s="58"/>
-      <c r="D97" s="58"/>
-      <c r="E97" s="58"/>
-      <c r="F97" s="58"/>
-      <c r="G97" s="58"/>
-      <c r="H97" s="58"/>
-      <c r="I97" s="58"/>
+      <c r="B97" s="59"/>
+      <c r="C97" s="59"/>
+      <c r="D97" s="59"/>
+      <c r="E97" s="59"/>
+      <c r="F97" s="59"/>
+      <c r="G97" s="59"/>
+      <c r="H97" s="59"/>
+      <c r="I97" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="98">
-      <c r="B98" s="58"/>
-      <c r="C98" s="58"/>
-      <c r="D98" s="58"/>
-      <c r="E98" s="58"/>
-      <c r="F98" s="58"/>
-      <c r="G98" s="58"/>
-      <c r="H98" s="58"/>
-      <c r="I98" s="58"/>
+      <c r="B98" s="59"/>
+      <c r="C98" s="59"/>
+      <c r="D98" s="59"/>
+      <c r="E98" s="59"/>
+      <c r="F98" s="59"/>
+      <c r="G98" s="59"/>
+      <c r="H98" s="59"/>
+      <c r="I98" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="99">
-      <c r="B99" s="58"/>
-      <c r="C99" s="58"/>
-      <c r="D99" s="58"/>
-      <c r="E99" s="58"/>
-      <c r="F99" s="58"/>
-      <c r="G99" s="58"/>
-      <c r="H99" s="58"/>
-      <c r="I99" s="58"/>
+      <c r="B99" s="59"/>
+      <c r="C99" s="59"/>
+      <c r="D99" s="59"/>
+      <c r="E99" s="59"/>
+      <c r="F99" s="59"/>
+      <c r="G99" s="59"/>
+      <c r="H99" s="59"/>
+      <c r="I99" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="100">
-      <c r="B100" s="58"/>
-      <c r="C100" s="58"/>
-      <c r="D100" s="58"/>
-      <c r="E100" s="58"/>
-      <c r="F100" s="58"/>
-      <c r="G100" s="58"/>
-      <c r="H100" s="58"/>
-      <c r="I100" s="58"/>
+      <c r="B100" s="59"/>
+      <c r="C100" s="59"/>
+      <c r="D100" s="59"/>
+      <c r="E100" s="59"/>
+      <c r="F100" s="59"/>
+      <c r="G100" s="59"/>
+      <c r="H100" s="59"/>
+      <c r="I100" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="101">
-      <c r="B101" s="58"/>
-      <c r="C101" s="58"/>
-      <c r="D101" s="58"/>
-      <c r="E101" s="58"/>
-      <c r="F101" s="58"/>
-      <c r="G101" s="58"/>
-      <c r="H101" s="58"/>
-      <c r="I101" s="58"/>
+      <c r="B101" s="59"/>
+      <c r="C101" s="59"/>
+      <c r="D101" s="59"/>
+      <c r="E101" s="59"/>
+      <c r="F101" s="59"/>
+      <c r="G101" s="59"/>
+      <c r="H101" s="59"/>
+      <c r="I101" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="102">
-      <c r="B102" s="58"/>
-      <c r="C102" s="58"/>
-      <c r="D102" s="58"/>
-      <c r="E102" s="58"/>
-      <c r="F102" s="58"/>
-      <c r="G102" s="58"/>
-      <c r="H102" s="58"/>
-      <c r="I102" s="58"/>
+      <c r="B102" s="59"/>
+      <c r="C102" s="59"/>
+      <c r="D102" s="59"/>
+      <c r="E102" s="59"/>
+      <c r="F102" s="59"/>
+      <c r="G102" s="59"/>
+      <c r="H102" s="59"/>
+      <c r="I102" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="103">
-      <c r="B103" s="58"/>
-      <c r="C103" s="58"/>
-      <c r="D103" s="58"/>
-      <c r="E103" s="58"/>
-      <c r="F103" s="58"/>
-      <c r="G103" s="58"/>
-      <c r="H103" s="58"/>
-      <c r="I103" s="58"/>
+      <c r="B103" s="59"/>
+      <c r="C103" s="59"/>
+      <c r="D103" s="59"/>
+      <c r="E103" s="59"/>
+      <c r="F103" s="59"/>
+      <c r="G103" s="59"/>
+      <c r="H103" s="59"/>
+      <c r="I103" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="104">
-      <c r="B104" s="58"/>
-      <c r="C104" s="58"/>
-      <c r="D104" s="58"/>
-      <c r="E104" s="58"/>
-      <c r="F104" s="58"/>
-      <c r="G104" s="58"/>
-      <c r="H104" s="58"/>
-      <c r="I104" s="58"/>
+      <c r="B104" s="59"/>
+      <c r="C104" s="59"/>
+      <c r="D104" s="59"/>
+      <c r="E104" s="59"/>
+      <c r="F104" s="59"/>
+      <c r="G104" s="59"/>
+      <c r="H104" s="59"/>
+      <c r="I104" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="105">
-      <c r="B105" s="58"/>
-      <c r="C105" s="58"/>
-      <c r="D105" s="58"/>
-      <c r="E105" s="58"/>
-      <c r="F105" s="58"/>
-      <c r="G105" s="58"/>
-      <c r="H105" s="58"/>
-      <c r="I105" s="58"/>
+      <c r="B105" s="59"/>
+      <c r="C105" s="59"/>
+      <c r="D105" s="59"/>
+      <c r="E105" s="59"/>
+      <c r="F105" s="59"/>
+      <c r="G105" s="59"/>
+      <c r="H105" s="59"/>
+      <c r="I105" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="106">
-      <c r="B106" s="58"/>
-      <c r="C106" s="58"/>
-      <c r="D106" s="58"/>
-      <c r="E106" s="58"/>
-      <c r="F106" s="58"/>
-      <c r="G106" s="58"/>
-      <c r="H106" s="58"/>
-      <c r="I106" s="58"/>
+      <c r="B106" s="59"/>
+      <c r="C106" s="59"/>
+      <c r="D106" s="59"/>
+      <c r="E106" s="59"/>
+      <c r="F106" s="59"/>
+      <c r="G106" s="59"/>
+      <c r="H106" s="59"/>
+      <c r="I106" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="107">
-      <c r="B107" s="58"/>
-      <c r="C107" s="58"/>
-      <c r="D107" s="58"/>
-      <c r="E107" s="58"/>
-      <c r="F107" s="58"/>
-      <c r="G107" s="58"/>
-      <c r="H107" s="58"/>
-      <c r="I107" s="58"/>
+      <c r="B107" s="59"/>
+      <c r="C107" s="59"/>
+      <c r="D107" s="59"/>
+      <c r="E107" s="59"/>
+      <c r="F107" s="59"/>
+      <c r="G107" s="59"/>
+      <c r="H107" s="59"/>
+      <c r="I107" s="59"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="108">
-      <c r="B108" s="58"/>
-      <c r="C108" s="58"/>
-      <c r="D108" s="58"/>
-      <c r="E108" s="58"/>
-      <c r="F108" s="58"/>
-      <c r="G108" s="58"/>
-      <c r="H108" s="58"/>
-      <c r="I108" s="58"/>
+      <c r="B108" s="59"/>
+      <c r="C108" s="59"/>
+      <c r="D108" s="59"/>
+      <c r="E108" s="59"/>
+      <c r="F108" s="59"/>
+      <c r="G108" s="59"/>
+      <c r="H108" s="59"/>
+      <c r="I108" s="59"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="109">
+      <c r="B109" s="59"/>
+      <c r="C109" s="59"/>
+      <c r="D109" s="59"/>
+      <c r="E109" s="59"/>
+      <c r="F109" s="59"/>
+      <c r="G109" s="59"/>
+      <c r="H109" s="59"/>
+      <c r="I109" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2065,223 +2095,223 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.0196078431373"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.0666666666667"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.8627450980392"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.4078431372549"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.843137254902"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="40.6352941176471"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.2039215686274"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.9882352941176"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="41.4509803921569"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.0196078431373"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="14.8313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="12.0196078431373"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.5921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7725490196078"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.3333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.0509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="25.1960784313725"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.243137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.7490196078431"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.3960784313725"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="42.0745098039216"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="8.5921568627451"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.0666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.5921568627451"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="2">
       <c r="B2" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="5">
-      <c r="A5" s="67" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" s="67" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" s="67" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" s="67" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" s="67" t="s">
-        <v>78</v>
-      </c>
-      <c r="F5" s="67" t="s">
+      <c r="A5" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="68" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="67" t="s">
-        <v>79</v>
-      </c>
-      <c r="H5" s="67" t="s">
+      <c r="G5" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="67" t="s">
-        <v>80</v>
-      </c>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
-      <c r="M5" s="67"/>
+      <c r="I5" s="68" t="s">
+        <v>86</v>
+      </c>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="6">
-      <c r="A6" s="67" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="67" t="s">
-        <v>82</v>
-      </c>
-      <c r="C6" s="67" t="s">
-        <v>83</v>
-      </c>
-      <c r="D6" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="67" t="s">
-        <v>85</v>
-      </c>
-      <c r="F6" s="67" t="s">
-        <v>86</v>
-      </c>
-      <c r="G6" s="67" t="s">
+      <c r="A6" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="H6" s="67" t="s">
+      <c r="B6" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="I6" s="67" t="s">
+      <c r="C6" s="68" t="s">
         <v>89</v>
       </c>
+      <c r="D6" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>92</v>
+      </c>
+      <c r="G6" s="68" t="s">
+        <v>93</v>
+      </c>
+      <c r="H6" s="68" t="s">
+        <v>94</v>
+      </c>
+      <c r="I6" s="68" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="B7" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" s="69" t="s">
+      <c r="B7" s="69" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="68" t="s">
-        <v>91</v>
-      </c>
-      <c r="E7" s="70" t="s">
-        <v>92</v>
-      </c>
-      <c r="F7" s="69" t="s">
+      <c r="D7" s="69" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="71" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="69" t="s">
-        <v>93</v>
-      </c>
-      <c r="H7" s="69" t="s">
-        <v>94</v>
-      </c>
-      <c r="I7" s="71" t="s">
-        <v>95</v>
+      <c r="G7" s="70" t="s">
+        <v>99</v>
+      </c>
+      <c r="H7" s="70" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="72" t="s">
+        <v>101</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
-      <c r="B8" s="68" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" s="69" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" s="68" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="68" t="s">
-        <v>99</v>
-      </c>
-      <c r="F8" s="68" t="s">
-        <v>100</v>
-      </c>
-      <c r="H8" s="69" t="s">
-        <v>101</v>
-      </c>
-      <c r="I8" s="71" t="s">
+      <c r="B8" s="69" t="s">
         <v>102</v>
       </c>
+      <c r="C8" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="69" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="69" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="69" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" s="70" t="s">
+        <v>107</v>
+      </c>
+      <c r="I8" s="72" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="9">
-      <c r="B9" s="68" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" s="69" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" s="68" t="s">
-        <v>105</v>
-      </c>
-      <c r="E9" s="70" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="68" t="s">
-        <v>107</v>
-      </c>
-      <c r="I9" s="71" t="s">
-        <v>108</v>
+      <c r="B9" s="69" t="s">
+        <v>109</v>
+      </c>
+      <c r="C9" s="70" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="69" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" s="71" t="s">
+        <v>112</v>
+      </c>
+      <c r="F9" s="69" t="s">
+        <v>113</v>
+      </c>
+      <c r="I9" s="72" t="s">
+        <v>114</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="10">
-      <c r="B10" s="69" t="s">
+      <c r="B10" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="69" t="s">
-        <v>109</v>
-      </c>
-      <c r="I10" s="71" t="s">
-        <v>110</v>
+      <c r="C10" s="70" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" s="72" t="s">
+        <v>116</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="11">
-      <c r="B11" s="69" t="s">
-        <v>111</v>
-      </c>
-      <c r="C11" s="69" t="s">
-        <v>112</v>
-      </c>
-      <c r="I11" s="72" t="s">
-        <v>113</v>
+      <c r="B11" s="70" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="70" t="s">
+        <v>118</v>
+      </c>
+      <c r="I11" s="73" t="s">
+        <v>119</v>
       </c>
       <c r="J11" s="0" t="n">
         <v>51</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="12">
-      <c r="B12" s="69" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12" s="69" t="s">
-        <v>115</v>
-      </c>
-      <c r="I12" s="72" t="s">
-        <v>116</v>
+      <c r="B12" s="70" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="70" t="s">
+        <v>121</v>
+      </c>
+      <c r="I12" s="73" t="s">
+        <v>122</v>
       </c>
       <c r="J12" s="0" t="n">
         <v>50</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="13">
-      <c r="B13" s="69" t="s">
-        <v>117</v>
-      </c>
-      <c r="I13" s="72" t="s">
-        <v>118</v>
+      <c r="B13" s="70" t="s">
+        <v>123</v>
+      </c>
+      <c r="I13" s="73" t="s">
+        <v>124</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="14">
-      <c r="B14" s="69" t="s">
-        <v>119</v>
-      </c>
-      <c r="I14" s="72" t="s">
-        <v>120</v>
+      <c r="B14" s="70" t="s">
+        <v>125</v>
+      </c>
+      <c r="I14" s="73" t="s">
+        <v>126</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
-      <c r="B18" s="69" t="s">
+      <c r="B18" s="70" t="s">
         <v>2</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
-      <c r="B19" s="68" t="s">
-        <v>74</v>
+      <c r="B19" s="69" t="s">
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
-      <c r="B20" s="70" t="s">
-        <v>121</v>
+      <c r="B20" s="71" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>